<commit_message>
Need to change FTTH WDM 100 in all excel files
</commit_message>
<xml_diff>
--- a/tumlknexpectimax/excel_data/input_data_NY_business.xlsx
+++ b/tumlknexpectimax/excel_data/input_data_NY_business.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmadzay\LRZ Sync+Share\PycharmProjects\mt_branch_new_code\tumlknexpectimax\tumlknexpectimax\excel_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="708" windowWidth="13680" windowHeight="11196" tabRatio="847"/>
+    <workbookView xWindow="480" yWindow="705" windowWidth="13680" windowHeight="11190" tabRatio="847" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
@@ -31,7 +26,7 @@
     <sheet name="FTTB_Hybridpon_100" sheetId="19" r:id="rId17"/>
     <sheet name="MIG_MATRIX" sheetId="11" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -41,7 +36,7 @@
     <author>Patri, Sai Kireet</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0">
+    <comment ref="H4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0">
+    <comment ref="H6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="0" shapeId="0">
+    <comment ref="H7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0">
+    <comment ref="B8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -547,7 +542,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000000%"/>
   </numFmts>
@@ -772,9 +767,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -801,6 +796,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -920,7 +916,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F92B-4BDB-8C8A-80B4841F7958}"/>
             </c:ext>
@@ -1036,7 +1032,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F92B-4BDB-8C8A-80B4841F7958}"/>
             </c:ext>
@@ -1152,7 +1148,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-F92B-4BDB-8C8A-80B4841F7958}"/>
             </c:ext>
@@ -1268,7 +1264,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-F92B-4BDB-8C8A-80B4841F7958}"/>
             </c:ext>
@@ -1284,11 +1280,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="159841280"/>
-        <c:axId val="83707008"/>
+        <c:axId val="61426176"/>
+        <c:axId val="60879936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="159841280"/>
+        <c:axId val="61426176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1310,13 +1306,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83707008"/>
+        <c:crossAx val="60879936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1324,7 +1321,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83707008"/>
+        <c:axId val="60879936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,19 +1344,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159841280"/>
+        <c:crossAx val="61426176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1375,9 +1374,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1404,6 +1403,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1485,51 +1485,51 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>20000</c:v>
+                  <c:v>54093.51440637085</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19283.042118970367</c:v>
+                  <c:v>28924.563178455599</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43709.823692218881</c:v>
+                  <c:v>65564.735538328358</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44248.4220525376</c:v>
+                  <c:v>66372.633078806393</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10540.776519765759</c:v>
+                  <c:v>15811.164779648698</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11938.918689039821</c:v>
+                  <c:v>17908.3780335597</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50983.71612182937</c:v>
+                  <c:v>76475.574182744094</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>47726.863400003029</c:v>
+                  <c:v>71590.2951000045</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>48220.289169209609</c:v>
+                  <c:v>72330.433753814403</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37682.867713520049</c:v>
+                  <c:v>56524.301570279997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44827.8721002112</c:v>
+                  <c:v>67241.808150316792</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12139.814930199653</c:v>
+                  <c:v>18209.722395299548</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>47419.574760442287</c:v>
+                  <c:v>71129.362140663448</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>50088.476920599649</c:v>
+                  <c:v>75132.715380899404</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3350-48DF-A99C-6FB4100C1476}"/>
             </c:ext>
@@ -1544,11 +1544,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="162980352"/>
-        <c:axId val="83711040"/>
+        <c:axId val="61519360"/>
+        <c:axId val="60882240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="162980352"/>
+        <c:axId val="61519360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,7 +1558,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83711040"/>
+        <c:crossAx val="60882240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1566,7 +1566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83711040"/>
+        <c:axId val="60882240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,13 +1589,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162980352"/>
+        <c:crossAx val="61519360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1613,9 +1614,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1780,7 +1781,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-41B7-4161-A3FD-A74535C0EF25}"/>
             </c:ext>
@@ -1909,7 +1910,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-41B7-4161-A3FD-A74535C0EF25}"/>
             </c:ext>
@@ -1924,11 +1925,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="163074560"/>
-        <c:axId val="84140032"/>
+        <c:axId val="63198720"/>
+        <c:axId val="61383808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="163074560"/>
+        <c:axId val="63198720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1945,10 +1946,10 @@
             <a:pPr>
               <a:defRPr sz="1200"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84140032"/>
+        <c:crossAx val="61383808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1956,7 +1957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84140032"/>
+        <c:axId val="61383808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1979,6 +1980,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1992,10 +1994,10 @@
             <a:pPr>
               <a:defRPr sz="1200"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="163074560"/>
+        <c:crossAx val="63198720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2011,7 +2013,7 @@
             <a:pPr>
               <a:defRPr sz="1400"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -2024,7 +2026,7 @@
             <a:pPr>
               <a:defRPr sz="1400"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -2053,9 +2055,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2232,7 +2234,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-111F-41C6-80A4-5A2D634965A5}"/>
             </c:ext>
@@ -2397,7 +2399,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-111F-41C6-80A4-5A2D634965A5}"/>
             </c:ext>
@@ -2562,7 +2564,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-111F-41C6-80A4-5A2D634965A5}"/>
             </c:ext>
@@ -2577,11 +2579,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82387456"/>
-        <c:axId val="127755392"/>
+        <c:axId val="63072768"/>
+        <c:axId val="61386112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82387456"/>
+        <c:axId val="63072768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2591,7 +2593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127755392"/>
+        <c:crossAx val="61386112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2599,7 +2601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127755392"/>
+        <c:axId val="61386112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2610,7 +2612,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82387456"/>
+        <c:crossAx val="63072768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2651,7 +2653,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2692,7 +2694,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2733,7 +2735,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2774,7 +2776,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2838,7 +2840,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2871,26 +2873,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2923,23 +2908,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3118,31 +3086,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="S3" sqref="S3:V15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
-    <col min="9" max="10" width="19.109375" customWidth="1"/>
+    <col min="1" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" customWidth="1"/>
-    <col min="15" max="15" width="22.109375" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" customWidth="1"/>
-    <col min="17" max="18" width="11.6640625" customWidth="1"/>
-    <col min="24" max="24" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" customWidth="1"/>
+    <col min="17" max="18" width="11.7109375" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="9" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3216,7 +3184,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
@@ -3256,7 +3224,7 @@
       </c>
       <c r="X2" s="13"/>
     </row>
-    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>73</v>
       </c>
@@ -3336,7 +3304,7 @@
         <v>291788.63717996189</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>66</v>
       </c>
@@ -3416,7 +3384,7 @@
         <v>277824.94829107303</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>67</v>
       </c>
@@ -3492,7 +3460,7 @@
         <v>227248.16613108691</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
@@ -3572,7 +3540,7 @@
         <v>409874.16613108688</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>69</v>
       </c>
@@ -3652,7 +3620,7 @@
         <v>461966.14829107304</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>70</v>
       </c>
@@ -3730,7 +3698,7 @@
         <v>326492.94829107303</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>71</v>
       </c>
@@ -3808,7 +3776,7 @@
         <v>247053.24829107302</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>72</v>
       </c>
@@ -3885,7 +3853,7 @@
         <v>338458.16613108688</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
@@ -3963,7 +3931,7 @@
         <v>246300.33066481428</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>75</v>
       </c>
@@ -4041,7 +4009,7 @@
         <v>249323.97727255611</v>
       </c>
     </row>
-    <row r="13" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
@@ -4119,7 +4087,7 @@
         <v>525612.57727255614</v>
       </c>
     </row>
-    <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>77</v>
       </c>
@@ -4197,7 +4165,7 @@
         <v>443647.77727255609</v>
       </c>
     </row>
-    <row r="15" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>78</v>
       </c>
@@ -4275,13 +4243,13 @@
         <v>384812.57727255614</v>
       </c>
     </row>
-    <row r="27" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="17:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="Q27">
         <f>0.02/1000</f>
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="42" spans="18:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="18:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="R42" s="5" t="s">
         <v>52</v>
       </c>
@@ -4295,12 +4263,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="18:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="18:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="S43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="18:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="18:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="R44" t="s">
         <v>55</v>
       </c>
@@ -4320,7 +4288,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="18:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="18:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="S45" t="s">
         <v>57</v>
       </c>
@@ -4331,7 +4299,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="18:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="18:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="R46" t="s">
         <v>60</v>
       </c>
@@ -4367,7 +4335,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5816,7 +5784,7 @@
       <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -7265,9 +7233,9 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="16.88671875" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -8717,7 +8685,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -10166,7 +10134,7 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -11615,7 +11583,7 @@
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -13064,7 +13032,7 @@
       <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -14513,7 +14481,7 @@
       <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -15962,23 +15930,23 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" customWidth="1"/>
-    <col min="15" max="15" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -16749,15 +16717,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="39.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -16773,7 +16741,8 @@
         <v>23</v>
       </c>
       <c r="B2" s="12">
-        <v>20000</v>
+        <f>AVERAGE(B3:B15)</f>
+        <v>54093.51440637085</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -16781,7 +16750,8 @@
         <v>73</v>
       </c>
       <c r="B3" s="12">
-        <v>19283.042118970367</v>
+        <f>1.5*19283.0421189704</f>
+        <v>28924.563178455599</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -16789,7 +16759,8 @@
         <v>66</v>
       </c>
       <c r="B4" s="12">
-        <v>43709.823692218881</v>
+        <f>1.5*43709.8236922189</f>
+        <v>65564.735538328358</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -16797,7 +16768,8 @@
         <v>67</v>
       </c>
       <c r="B5" s="12">
-        <v>44248.4220525376</v>
+        <f>1.5*44248.4220525376</f>
+        <v>66372.633078806393</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -16805,7 +16777,8 @@
         <v>68</v>
       </c>
       <c r="B6" s="12">
-        <v>10540.776519765759</v>
+        <f>1.5*10540.7765197658</f>
+        <v>15811.164779648698</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -16813,7 +16786,8 @@
         <v>69</v>
       </c>
       <c r="B7" s="12">
-        <v>11938.918689039821</v>
+        <f>1.5*11938.9186890398</f>
+        <v>17908.3780335597</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -16821,7 +16795,8 @@
         <v>70</v>
       </c>
       <c r="B8" s="12">
-        <v>50983.71612182937</v>
+        <f>1.5*50983.7161218294</f>
+        <v>76475.574182744094</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -16829,7 +16804,8 @@
         <v>71</v>
       </c>
       <c r="B9" s="12">
-        <v>47726.863400003029</v>
+        <f>1.5*47726.863400003</f>
+        <v>71590.2951000045</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -16837,7 +16813,8 @@
         <v>72</v>
       </c>
       <c r="B10" s="12">
-        <v>48220.289169209609</v>
+        <f>1.5*48220.2891692096</f>
+        <v>72330.433753814403</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -16845,7 +16822,8 @@
         <v>74</v>
       </c>
       <c r="B11" s="12">
-        <v>37682.867713520049</v>
+        <f>1.5*37682.86771352</f>
+        <v>56524.301570279997</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -16853,7 +16831,8 @@
         <v>75</v>
       </c>
       <c r="B12" s="12">
-        <v>44827.8721002112</v>
+        <f>1.5*44827.8721002112</f>
+        <v>67241.808150316792</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -16861,7 +16840,8 @@
         <v>76</v>
       </c>
       <c r="B13" s="12">
-        <v>12139.814930199653</v>
+        <f>1.5*12139.8149301997</f>
+        <v>18209.722395299548</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -16869,7 +16849,8 @@
         <v>77</v>
       </c>
       <c r="B14" s="12">
-        <v>47419.574760442287</v>
+        <f>1.5*47419.5747604423</f>
+        <v>71129.362140663448</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -16877,7 +16858,8 @@
         <v>78</v>
       </c>
       <c r="B15" s="12">
-        <v>50088.476920599649</v>
+        <f>1.5*50088.4769205996</f>
+        <v>75132.715380899404</v>
       </c>
     </row>
   </sheetData>
@@ -16898,22 +16880,22 @@
       <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
-    <col min="34" max="34" width="17.88671875" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="34" max="34" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -16993,7 +16975,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2018</v>
       </c>
@@ -17041,31 +17023,31 @@
       </c>
       <c r="U2" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V2" s="11">
         <f>O2-U2</f>
-        <v>-46836.476920599649</v>
+        <v>-71880.715380899404</v>
       </c>
       <c r="W2" s="11">
         <f>P2-U2</f>
-        <v>-46836.476920599649</v>
+        <v>-71880.715380899404</v>
       </c>
       <c r="X2" s="11">
         <f t="shared" ref="X2:X22" si="1">Q2-U2</f>
-        <v>-46836.476920599649</v>
+        <v>-71880.715380899404</v>
       </c>
       <c r="Y2" s="11">
         <f>R2-$U2</f>
-        <v>-47196.476920599649</v>
+        <v>-72240.715380899404</v>
       </c>
       <c r="Z2" s="11">
         <f>S2-$U2</f>
-        <v>-47196.476920599649</v>
+        <v>-72240.715380899404</v>
       </c>
       <c r="AA2" s="11">
         <f>T2-$U2</f>
-        <v>-47196.476920599649</v>
+        <v>-72240.715380899404</v>
       </c>
       <c r="AB2" s="11">
         <f>1/POWER(1+$L$25,N2-2018)</f>
@@ -17073,30 +17055,30 @@
       </c>
       <c r="AC2" s="12">
         <f>V2*AB2</f>
-        <v>-46836.476920599649</v>
+        <v>-71880.715380899404</v>
       </c>
       <c r="AD2" s="12">
         <f>W2*AB2</f>
-        <v>-46836.476920599649</v>
+        <v>-71880.715380899404</v>
       </c>
       <c r="AE2" s="12">
         <f>X2*AB2</f>
-        <v>-46836.476920599649</v>
+        <v>-71880.715380899404</v>
       </c>
       <c r="AF2" s="12">
         <f>Y2*$AB2</f>
-        <v>-47196.476920599649</v>
+        <v>-72240.715380899404</v>
       </c>
       <c r="AG2" s="12">
         <f>Z2*$AB2</f>
-        <v>-47196.476920599649</v>
+        <v>-72240.715380899404</v>
       </c>
       <c r="AH2" s="12">
         <f>AA2*$AB2</f>
-        <v>-47196.476920599649</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+        <v>-72240.715380899404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2019</v>
       </c>
@@ -17143,31 +17125,31 @@
       </c>
       <c r="U3" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V3" s="11">
         <f t="shared" ref="V3:V22" si="8">O3-U3</f>
-        <v>-45816.476920599649</v>
+        <v>-70860.715380899404</v>
       </c>
       <c r="W3" s="11">
         <f t="shared" ref="W3:W22" si="9">P3-U3</f>
-        <v>-45672.476920599649</v>
+        <v>-70716.715380899404</v>
       </c>
       <c r="X3" s="11">
         <f t="shared" si="1"/>
-        <v>-44052.476920599649</v>
+        <v>-69096.715380899404</v>
       </c>
       <c r="Y3" s="11">
         <f t="shared" ref="Y3:Y22" si="10">R3-$U3</f>
-        <v>-46260.476920599649</v>
+        <v>-71304.715380899404</v>
       </c>
       <c r="Z3" s="11">
         <f t="shared" ref="Z3:Z22" si="11">S3-$U3</f>
-        <v>-46128.476920599649</v>
+        <v>-71172.715380899404</v>
       </c>
       <c r="AA3" s="11">
         <f t="shared" ref="AA3:AA22" si="12">T3-$U3</f>
-        <v>-44664.476920599649</v>
+        <v>-69708.715380899404</v>
       </c>
       <c r="AB3" s="11">
         <f t="shared" ref="AB3:AB22" si="13">1/POWER(1+$L$25,N3-2018)</f>
@@ -17175,30 +17157,30 @@
       </c>
       <c r="AC3" s="12">
         <f t="shared" ref="AC3:AC22" si="14">V3*AB3</f>
-        <v>-41651.342655090586</v>
+        <v>-64418.832164454005</v>
       </c>
       <c r="AD3" s="12">
         <f t="shared" ref="AD3:AD22" si="15">W3*AB3</f>
-        <v>-41520.433564181498</v>
+        <v>-64287.923073544909</v>
       </c>
       <c r="AE3" s="12">
         <f t="shared" ref="AE3:AE22" si="16">X3*AB3</f>
-        <v>-40047.706291454226</v>
+        <v>-62815.195800817637</v>
       </c>
       <c r="AF3" s="12">
         <f t="shared" ref="AF3:AF22" si="17">Y3*$AB3</f>
-        <v>-42054.979018726954</v>
+        <v>-64822.468528090365</v>
       </c>
       <c r="AG3" s="12">
         <f t="shared" ref="AG3:AG22" si="18">Z3*$AB3</f>
-        <v>-41934.979018726954</v>
+        <v>-64702.468528090365</v>
       </c>
       <c r="AH3" s="12">
         <f t="shared" ref="AH3:AH22" si="19">AA3*$AB3</f>
-        <v>-40604.069927817858</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+        <v>-63371.559437181277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2020</v>
       </c>
@@ -17254,31 +17236,31 @@
       </c>
       <c r="U4" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V4" s="11">
         <f t="shared" si="8"/>
-        <v>-44316.476920599649</v>
+        <v>-69360.715380899404</v>
       </c>
       <c r="W4" s="11">
         <f t="shared" si="9"/>
-        <v>-43944.476920599649</v>
+        <v>-68988.715380899404</v>
       </c>
       <c r="X4" s="11">
         <f t="shared" si="1"/>
-        <v>-38580.476920599649</v>
+        <v>-63624.715380899404</v>
       </c>
       <c r="Y4" s="11">
         <f t="shared" si="10"/>
-        <v>-44904.476920599649</v>
+        <v>-69948.715380899404</v>
       </c>
       <c r="Z4" s="11">
         <f t="shared" si="11"/>
-        <v>-44568.476920599649</v>
+        <v>-69612.715380899404</v>
       </c>
       <c r="AA4" s="11">
         <f t="shared" si="12"/>
-        <v>-39756.476920599649</v>
+        <v>-64800.715380899404</v>
       </c>
       <c r="AB4" s="11">
         <f t="shared" si="13"/>
@@ -17286,30 +17268,30 @@
       </c>
       <c r="AC4" s="12">
         <f t="shared" si="14"/>
-        <v>-36625.187537685655</v>
+        <v>-57322.905273470577</v>
       </c>
       <c r="AD4" s="12">
         <f t="shared" si="15"/>
-        <v>-36317.749521156729</v>
+        <v>-57015.467256941651</v>
       </c>
       <c r="AE4" s="12">
         <f t="shared" si="16"/>
-        <v>-31884.691669917062</v>
+        <v>-52582.409405701983</v>
       </c>
       <c r="AF4" s="12">
         <f t="shared" si="17"/>
-        <v>-37111.1379509088</v>
+        <v>-57808.855686693714</v>
       </c>
       <c r="AG4" s="12">
         <f t="shared" si="18"/>
-        <v>-36833.45200049557</v>
+        <v>-57531.169736280492</v>
       </c>
       <c r="AH4" s="12">
         <f t="shared" si="19"/>
-        <v>-32856.592496363344</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+        <v>-53554.310232148266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2021</v>
       </c>
@@ -17366,31 +17348,31 @@
       </c>
       <c r="U5" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V5" s="11">
         <f t="shared" si="8"/>
-        <v>-42264.476920599649</v>
+        <v>-67308.715380899404</v>
       </c>
       <c r="W5" s="11">
         <f t="shared" si="9"/>
-        <v>-41424.476920599649</v>
+        <v>-66468.715380899404</v>
       </c>
       <c r="X5" s="11">
         <f t="shared" si="1"/>
-        <v>-27852.476920599649</v>
+        <v>-52896.715380899404</v>
       </c>
       <c r="Y5" s="11">
         <f t="shared" si="10"/>
-        <v>-43056.476920599649</v>
+        <v>-68100.715380899404</v>
       </c>
       <c r="Z5" s="11">
         <f t="shared" si="11"/>
-        <v>-42312.476920599649</v>
+        <v>-67356.715380899404</v>
       </c>
       <c r="AA5" s="11">
         <f t="shared" si="12"/>
-        <v>-30108.476920599649</v>
+        <v>-55152.715380899404</v>
       </c>
       <c r="AB5" s="11">
         <f t="shared" si="13"/>
@@ -17398,30 +17380,30 @@
       </c>
       <c r="AC5" s="12">
         <f t="shared" si="14"/>
-        <v>-31753.927062809646</v>
+        <v>-50570.034095341383</v>
       </c>
       <c r="AD5" s="12">
         <f t="shared" si="15"/>
-        <v>-31122.82263005232</v>
+        <v>-49938.929662584058</v>
       </c>
       <c r="AE5" s="12">
         <f t="shared" si="16"/>
-        <v>-20925.97815221611</v>
+        <v>-39742.085184747848</v>
       </c>
       <c r="AF5" s="12">
         <f t="shared" si="17"/>
-        <v>-32348.968385123695</v>
+        <v>-51165.075417655433</v>
       </c>
       <c r="AG5" s="12">
         <f t="shared" si="18"/>
-        <v>-31789.990173252922</v>
+        <v>-50606.097205784659</v>
       </c>
       <c r="AH5" s="12">
         <f t="shared" si="19"/>
-        <v>-22620.944343050069</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+        <v>-41437.05137558181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2022</v>
       </c>
@@ -17478,31 +17460,31 @@
       </c>
       <c r="U6" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V6" s="11">
         <f t="shared" si="8"/>
-        <v>-39384.476920599649</v>
+        <v>-64428.715380899404</v>
       </c>
       <c r="W6" s="11">
         <f t="shared" si="9"/>
-        <v>-37860.476920599649</v>
+        <v>-62904.715380899404</v>
       </c>
       <c r="X6" s="11">
         <f t="shared" si="1"/>
-        <v>-6888.476920599649</v>
+        <v>-31932.715380899404</v>
       </c>
       <c r="Y6" s="11">
         <f t="shared" si="10"/>
-        <v>-40464.476920599649</v>
+        <v>-65508.715380899404</v>
       </c>
       <c r="Z6" s="11">
         <f t="shared" si="11"/>
-        <v>-39096.476920599649</v>
+        <v>-64140.715380899404</v>
       </c>
       <c r="AA6" s="11">
         <f t="shared" si="12"/>
-        <v>-11220.476920599649</v>
+        <v>-36264.715380899404</v>
       </c>
       <c r="AB6" s="11">
         <f t="shared" si="13"/>
@@ -17510,30 +17492,30 @@
       </c>
       <c r="AC6" s="12">
         <f t="shared" si="14"/>
-        <v>-26900.127669284637</v>
+        <v>-44005.679517040771</v>
       </c>
       <c r="AD6" s="12">
         <f t="shared" si="15"/>
-        <v>-25859.215163308272</v>
+        <v>-42964.767011064403</v>
       </c>
       <c r="AE6" s="12">
         <f t="shared" si="16"/>
-        <v>-4704.9224237413064</v>
+        <v>-21810.474271497435</v>
       </c>
       <c r="AF6" s="12">
         <f t="shared" si="17"/>
-        <v>-27637.782201078913</v>
+        <v>-44743.334048835044</v>
       </c>
       <c r="AG6" s="12">
         <f t="shared" si="18"/>
-        <v>-26703.4197941395</v>
+        <v>-43808.97164189563</v>
       </c>
       <c r="AH6" s="12">
         <f t="shared" si="19"/>
-        <v>-7663.7367123827926</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+        <v>-24769.288560138921</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2023</v>
       </c>
@@ -17590,31 +17572,31 @@
       </c>
       <c r="U7" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V7" s="11">
         <f t="shared" si="8"/>
-        <v>-35472.476920599649</v>
+        <v>-60516.715380899404</v>
       </c>
       <c r="W7" s="11">
         <f t="shared" si="9"/>
-        <v>-32820.476920599649</v>
+        <v>-57864.715380899404</v>
       </c>
       <c r="X7" s="11">
         <f t="shared" si="1"/>
-        <v>33119.523079400351</v>
+        <v>8075.2846191005956</v>
       </c>
       <c r="Y7" s="11">
         <f t="shared" si="10"/>
-        <v>-36960.476920599649</v>
+        <v>-62004.715380899404</v>
       </c>
       <c r="Z7" s="11">
         <f t="shared" si="11"/>
-        <v>-34584.476920599649</v>
+        <v>-59628.715380899404</v>
       </c>
       <c r="AA7" s="11">
         <f t="shared" si="12"/>
-        <v>24779.523079400351</v>
+        <v>-264.71538089940441</v>
       </c>
       <c r="AB7" s="11">
         <f t="shared" si="13"/>
@@ -17622,30 +17604,30 @@
       </c>
       <c r="AC7" s="12">
         <f t="shared" si="14"/>
-        <v>-22025.617301724073</v>
+        <v>-37576.118981502368</v>
       </c>
       <c r="AD7" s="12">
         <f t="shared" si="15"/>
-        <v>-20378.933952971194</v>
+        <v>-35929.43563274949</v>
       </c>
       <c r="AE7" s="12">
         <f t="shared" si="16"/>
-        <v>20564.618089549484</v>
+        <v>5014.1164097711853</v>
       </c>
       <c r="AF7" s="12">
         <f t="shared" si="17"/>
-        <v>-22949.548230436096</v>
+        <v>-38500.049910214395</v>
       </c>
       <c r="AG7" s="12">
         <f t="shared" si="18"/>
-        <v>-21474.239166847543</v>
+        <v>-37024.740846625842</v>
       </c>
       <c r="AH7" s="12">
         <f t="shared" si="19"/>
-        <v>15386.134255236131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+        <v>-164.36742454216633</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2024</v>
       </c>
@@ -17702,31 +17684,31 @@
       </c>
       <c r="U8" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V8" s="11">
         <f t="shared" si="8"/>
-        <v>-30084.476920599649</v>
+        <v>-55128.715380899404</v>
       </c>
       <c r="W8" s="11">
         <f t="shared" si="9"/>
-        <v>-25632.476920599649</v>
+        <v>-50676.715380899404</v>
       </c>
       <c r="X8" s="11">
         <f t="shared" si="1"/>
-        <v>106727.52307940036</v>
+        <v>81683.284619100596</v>
       </c>
       <c r="Y8" s="11">
         <f t="shared" si="10"/>
-        <v>-32088.476920599649</v>
+        <v>-57132.715380899404</v>
       </c>
       <c r="Z8" s="11">
         <f t="shared" si="11"/>
-        <v>-28092.476920599649</v>
+        <v>-53136.715380899404</v>
       </c>
       <c r="AA8" s="11">
         <f t="shared" si="12"/>
-        <v>91019.523079400358</v>
+        <v>65975.284619100596</v>
       </c>
       <c r="AB8" s="11">
         <f t="shared" si="13"/>
@@ -17734,30 +17716,30 @@
       </c>
       <c r="AC8" s="12">
         <f t="shared" si="14"/>
-        <v>-16981.902920983041</v>
+        <v>-31118.722629872402</v>
       </c>
       <c r="AD8" s="12">
         <f t="shared" si="15"/>
-        <v>-14468.864984383625</v>
+        <v>-28605.684693272986</v>
       </c>
       <c r="AE8" s="12">
         <f t="shared" si="16"/>
-        <v>60244.90439753433</v>
+        <v>46108.084688644965</v>
       </c>
       <c r="AF8" s="12">
         <f t="shared" si="17"/>
-        <v>-18113.108676810811</v>
+        <v>-32249.928385700172</v>
       </c>
       <c r="AG8" s="12">
         <f t="shared" si="18"/>
-        <v>-15857.470852315917</v>
+        <v>-29994.290561205278</v>
       </c>
       <c r="AH8" s="12">
         <f t="shared" si="19"/>
-        <v>51378.147904249599</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+        <v>37241.328195360235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2025</v>
       </c>
@@ -17813,31 +17795,31 @@
       </c>
       <c r="U9" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V9" s="11">
         <f t="shared" si="8"/>
-        <v>-22752.476920599649</v>
+        <v>-47796.715380899404</v>
       </c>
       <c r="W9" s="11">
         <f t="shared" si="9"/>
-        <v>-15540.476920599649</v>
+        <v>-40584.715380899404</v>
       </c>
       <c r="X9" s="11">
         <f t="shared" si="1"/>
-        <v>231671.52307940036</v>
+        <v>206627.2846191006</v>
       </c>
       <c r="Y9" s="11">
         <f t="shared" si="10"/>
-        <v>-25500.476920599649</v>
+        <v>-50544.715380899404</v>
       </c>
       <c r="Z9" s="11">
         <f t="shared" si="11"/>
-        <v>-19020.476920599649</v>
+        <v>-44064.715380899404</v>
       </c>
       <c r="AA9" s="11">
         <f t="shared" si="12"/>
-        <v>203495.52307940036</v>
+        <v>178451.2846191006</v>
       </c>
       <c r="AB9" s="11">
         <f t="shared" si="13"/>
@@ -17845,30 +17827,30 @@
       </c>
       <c r="AC9" s="12">
         <f t="shared" si="14"/>
-        <v>-11675.618241662494</v>
+        <v>-24527.272522471001</v>
       </c>
       <c r="AD9" s="12">
         <f t="shared" si="15"/>
-        <v>-7974.7218929826395</v>
+        <v>-20826.376173791148</v>
       </c>
       <c r="AE9" s="12">
         <f t="shared" si="16"/>
-        <v>118884.12283106676</v>
+        <v>106032.46855025826</v>
       </c>
       <c r="AF9" s="12">
         <f t="shared" si="17"/>
-        <v>-13085.776750560475</v>
+        <v>-25937.431031368982</v>
       </c>
       <c r="AG9" s="12">
         <f t="shared" si="18"/>
-        <v>-9760.5121444254983</v>
+        <v>-22612.166425234005</v>
       </c>
       <c r="AH9" s="12">
         <f t="shared" si="19"/>
-        <v>104425.37969179839</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+        <v>91573.725410989864</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2026</v>
       </c>
@@ -17924,31 +17906,31 @@
       </c>
       <c r="U10" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V10" s="11">
         <f t="shared" si="8"/>
-        <v>-12768.476920599649</v>
+        <v>-37812.715380899404</v>
       </c>
       <c r="W10" s="11">
         <f t="shared" si="9"/>
-        <v>-1428.476920599649</v>
+        <v>-26472.715380899404</v>
       </c>
       <c r="X10" s="11">
         <f t="shared" si="1"/>
-        <v>412955.52307940036</v>
+        <v>387911.28461910062</v>
       </c>
       <c r="Y10" s="11">
         <f t="shared" si="10"/>
-        <v>-16536.476920599649</v>
+        <v>-41580.715380899404</v>
       </c>
       <c r="Z10" s="11">
         <f t="shared" si="11"/>
-        <v>-6324.476920599649</v>
+        <v>-31368.715380899404</v>
       </c>
       <c r="AA10" s="11">
         <f t="shared" si="12"/>
-        <v>366611.52307940036</v>
+        <v>341567.28461910062</v>
       </c>
       <c r="AB10" s="11">
         <f t="shared" si="13"/>
@@ -17956,30 +17938,30 @@
       </c>
       <c r="AC10" s="12">
         <f t="shared" si="14"/>
-        <v>-5956.5887174973832</v>
+        <v>-17639.910790959664</v>
       </c>
       <c r="AD10" s="12">
         <f t="shared" si="15"/>
-        <v>-666.3950259190093</v>
+        <v>-12349.717099381289</v>
       </c>
       <c r="AE10" s="12">
         <f t="shared" si="16"/>
-        <v>192646.79921491107</v>
+        <v>180963.47714144879</v>
       </c>
       <c r="AF10" s="12">
         <f t="shared" si="17"/>
-        <v>-7714.3885261276573</v>
+        <v>-19397.710599589936</v>
       </c>
       <c r="AG10" s="12">
         <f t="shared" si="18"/>
-        <v>-2950.4151594258628</v>
+        <v>-14633.737232888143</v>
       </c>
       <c r="AH10" s="12">
         <f t="shared" si="19"/>
-        <v>171026.98118647118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+        <v>159343.65911300891</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2027</v>
       </c>
@@ -18035,31 +18017,31 @@
       </c>
       <c r="U11" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V11" s="11">
         <f t="shared" si="8"/>
-        <v>695.52307940035098</v>
+        <v>-24348.715380899404</v>
       </c>
       <c r="W11" s="11">
         <f t="shared" si="9"/>
-        <v>18119.523079400351</v>
+        <v>-6924.7153808994044</v>
       </c>
       <c r="X11" s="11">
         <f t="shared" si="1"/>
-        <v>606647.5230794003</v>
+        <v>581603.28461910062</v>
       </c>
       <c r="Y11" s="11">
         <f t="shared" si="10"/>
-        <v>-4392.476920599649</v>
+        <v>-29436.715380899404</v>
       </c>
       <c r="Z11" s="11">
         <f t="shared" si="11"/>
-        <v>11291.523079400351</v>
+        <v>-13752.715380899404</v>
       </c>
       <c r="AA11" s="11">
         <f t="shared" si="12"/>
-        <v>540935.5230794003</v>
+        <v>515891.28461910062</v>
       </c>
       <c r="AB11" s="11">
         <f t="shared" si="13"/>
@@ -18067,30 +18049,30 @@
       </c>
       <c r="AC11" s="12">
         <f t="shared" si="14"/>
-        <v>294.96968149678543</v>
+        <v>-10326.232203468922</v>
       </c>
       <c r="AD11" s="12">
         <f t="shared" si="15"/>
-        <v>7684.4465840189578</v>
+        <v>-2936.7553009467506</v>
       </c>
       <c r="AE11" s="12">
         <f t="shared" si="16"/>
-        <v>257277.7697295406</v>
+        <v>246656.56784457492</v>
       </c>
       <c r="AF11" s="12">
         <f t="shared" si="17"/>
-        <v>-1862.8390007824166</v>
+        <v>-12484.040885748125</v>
       </c>
       <c r="AG11" s="12">
         <f t="shared" si="18"/>
-        <v>4788.7080457716329</v>
+        <v>-5832.4938391940759</v>
       </c>
       <c r="AH11" s="12">
         <f t="shared" si="19"/>
-        <v>229409.46703104788</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+        <v>218788.26514608221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2028</v>
       </c>
@@ -18147,31 +18129,31 @@
       </c>
       <c r="U12" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V12" s="11">
         <f t="shared" si="8"/>
-        <v>18683.523079400351</v>
+        <v>-6360.7153808994044</v>
       </c>
       <c r="W12" s="11">
         <f t="shared" si="9"/>
-        <v>44855.523079400351</v>
+        <v>19811.284619100596</v>
       </c>
       <c r="X12" s="11">
         <f t="shared" si="1"/>
-        <v>722939.5230794003</v>
+        <v>697895.28461910062</v>
       </c>
       <c r="Y12" s="11">
         <f t="shared" si="10"/>
-        <v>11783.523079400351</v>
+        <v>-13260.715380899404</v>
       </c>
       <c r="Z12" s="11">
         <f t="shared" si="11"/>
-        <v>35327.523079400351</v>
+        <v>10283.284619100596</v>
       </c>
       <c r="AA12" s="11">
         <f t="shared" si="12"/>
-        <v>645611.5230794003</v>
+        <v>620567.28461910062</v>
       </c>
       <c r="AB12" s="11">
         <f t="shared" si="13"/>
@@ -18179,30 +18161,30 @@
       </c>
       <c r="AC12" s="12">
         <f t="shared" si="14"/>
-        <v>7203.3069461645809</v>
+        <v>-2452.3311310769718</v>
       </c>
       <c r="AD12" s="12">
         <f t="shared" si="15"/>
-        <v>17293.74591711428</v>
+        <v>7638.1078398727259</v>
       </c>
       <c r="AE12" s="12">
         <f t="shared" si="16"/>
-        <v>278724.48178664868</v>
+        <v>269068.84370940714</v>
       </c>
       <c r="AF12" s="12">
         <f t="shared" si="17"/>
-        <v>4543.0582491008136</v>
+        <v>-5112.5798281407388</v>
       </c>
       <c r="AG12" s="12">
         <f t="shared" si="18"/>
-        <v>13620.289455429702</v>
+        <v>3964.6513781881504</v>
       </c>
       <c r="AH12" s="12">
         <f t="shared" si="19"/>
-        <v>248911.19030164188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+        <v>239255.55222440034</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2029</v>
       </c>
@@ -18258,31 +18240,31 @@
       </c>
       <c r="U13" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V13" s="11">
         <f t="shared" si="8"/>
-        <v>42491.523079400351</v>
+        <v>17447.284619100596</v>
       </c>
       <c r="W13" s="11">
         <f t="shared" si="9"/>
-        <v>80723.523079400358</v>
+        <v>55679.284619100596</v>
       </c>
       <c r="X13" s="11">
         <f t="shared" si="1"/>
-        <v>747863.5230794003</v>
+        <v>722819.28461910062</v>
       </c>
       <c r="Y13" s="11">
         <f t="shared" si="10"/>
-        <v>33215.523079400351</v>
+        <v>8171.2846191005956</v>
       </c>
       <c r="Z13" s="11">
         <f t="shared" si="11"/>
-        <v>67619.523079400358</v>
+        <v>42575.284619100596</v>
       </c>
       <c r="AA13" s="11">
         <f t="shared" si="12"/>
-        <v>668039.5230794003</v>
+        <v>642995.28461910062</v>
       </c>
       <c r="AB13" s="11">
         <f t="shared" si="13"/>
@@ -18290,30 +18272,30 @@
       </c>
       <c r="AC13" s="12">
         <f t="shared" si="14"/>
-        <v>14893.019619002604</v>
+        <v>6115.1668215102845</v>
       </c>
       <c r="AD13" s="12">
         <f t="shared" si="15"/>
-        <v>28293.102383975194</v>
+        <v>19515.249586482871</v>
       </c>
       <c r="AE13" s="12">
         <f t="shared" si="16"/>
-        <v>262121.60248399116</v>
+        <v>253343.74968649886</v>
       </c>
       <c r="AF13" s="12">
         <f t="shared" si="17"/>
-        <v>11641.83820741321</v>
+        <v>2863.9854099208901</v>
       </c>
       <c r="AG13" s="12">
         <f t="shared" si="18"/>
-        <v>23700.230325171029</v>
+        <v>14922.377527678707</v>
       </c>
       <c r="AH13" s="12">
         <f t="shared" si="19"/>
-        <v>234143.77745178851</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+        <v>225365.92465429622</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2030</v>
       </c>
@@ -18369,31 +18351,31 @@
       </c>
       <c r="U14" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V14" s="11">
         <f t="shared" si="8"/>
-        <v>73487.523079400358</v>
+        <v>48443.284619100596</v>
       </c>
       <c r="W14" s="11">
         <f t="shared" si="9"/>
-        <v>127631.52307940036</v>
+        <v>102587.2846191006</v>
       </c>
       <c r="X14" s="11">
         <f t="shared" si="1"/>
-        <v>749027.5230794003</v>
+        <v>723983.28461910062</v>
       </c>
       <c r="Y14" s="11">
         <f t="shared" si="10"/>
-        <v>61115.523079400351</v>
+        <v>36071.284619100596</v>
       </c>
       <c r="Z14" s="11">
         <f t="shared" si="11"/>
-        <v>109847.52307940036</v>
+        <v>84803.284619100596</v>
       </c>
       <c r="AA14" s="11">
         <f t="shared" si="12"/>
-        <v>669083.5230794003</v>
+        <v>644039.28461910062</v>
       </c>
       <c r="AB14" s="11">
         <f t="shared" si="13"/>
@@ -18401,30 +18383,30 @@
       </c>
       <c r="AC14" s="12">
         <f t="shared" si="14"/>
-        <v>23415.389570298037</v>
+        <v>15435.523390759561</v>
       </c>
       <c r="AD14" s="12">
         <f t="shared" si="15"/>
-        <v>40667.336564407582</v>
+        <v>32687.470384869106</v>
       </c>
       <c r="AE14" s="12">
         <f t="shared" si="16"/>
-        <v>238663.25216635229</v>
+        <v>230683.38598681384</v>
       </c>
       <c r="AF14" s="12">
         <f t="shared" si="17"/>
-        <v>19473.289093585503</v>
+        <v>11493.422914047031</v>
       </c>
       <c r="AG14" s="12">
         <f t="shared" si="18"/>
-        <v>35000.806102246599</v>
+        <v>27020.939922708127</v>
       </c>
       <c r="AH14" s="12">
         <f t="shared" si="19"/>
-        <v>213190.63007531554</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+        <v>205210.76389577711</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2031</v>
       </c>
@@ -18480,31 +18462,31 @@
       </c>
       <c r="U15" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V15" s="11">
         <f t="shared" si="8"/>
-        <v>113087.52307940036</v>
+        <v>88043.284619100596</v>
       </c>
       <c r="W15" s="11">
         <f t="shared" si="9"/>
-        <v>186851.52307940036</v>
+        <v>161807.2846191006</v>
       </c>
       <c r="X15" s="11">
         <f t="shared" si="1"/>
-        <v>749195.5230794003</v>
+        <v>724151.28461910062</v>
       </c>
       <c r="Y15" s="11">
         <f t="shared" si="10"/>
-        <v>96743.523079400358</v>
+        <v>71699.284619100596</v>
       </c>
       <c r="Z15" s="11">
         <f t="shared" si="11"/>
-        <v>163151.52307940036</v>
+        <v>138107.2846191006</v>
       </c>
       <c r="AA15" s="11">
         <f t="shared" si="12"/>
-        <v>669239.5230794003</v>
+        <v>644195.28461910062</v>
       </c>
       <c r="AB15" s="11">
         <f t="shared" si="13"/>
@@ -18512,30 +18494,30 @@
       </c>
       <c r="AC15" s="12">
         <f t="shared" si="14"/>
-        <v>32757.427228752869</v>
+        <v>25503.003429172437</v>
       </c>
       <c r="AD15" s="12">
         <f t="shared" si="15"/>
-        <v>54124.230535649906</v>
+        <v>46869.806736069477</v>
       </c>
       <c r="AE15" s="12">
         <f t="shared" si="16"/>
-        <v>217015.25649429785</v>
+        <v>209760.83269471745</v>
       </c>
       <c r="AF15" s="12">
         <f t="shared" si="17"/>
-        <v>28023.152606336444</v>
+        <v>20768.728806756015</v>
       </c>
       <c r="AG15" s="12">
         <f t="shared" si="18"/>
-        <v>47259.184735890405</v>
+        <v>40004.760936309976</v>
       </c>
       <c r="AH15" s="12">
         <f t="shared" si="19"/>
-        <v>193854.85134807124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+        <v>186600.42754849084</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2032</v>
       </c>
@@ -18591,31 +18573,31 @@
       </c>
       <c r="U16" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V16" s="11">
         <f t="shared" si="8"/>
-        <v>162299.52307940036</v>
+        <v>137255.2846191006</v>
       </c>
       <c r="W16" s="11">
         <f t="shared" si="9"/>
-        <v>258347.52307940036</v>
+        <v>233303.2846191006</v>
       </c>
       <c r="X16" s="11">
         <f t="shared" si="1"/>
-        <v>749315.5230794003</v>
+        <v>724271.28461910062</v>
       </c>
       <c r="Y16" s="11">
         <f t="shared" si="10"/>
-        <v>141023.52307940036</v>
+        <v>115979.2846191006</v>
       </c>
       <c r="Z16" s="11">
         <f t="shared" si="11"/>
-        <v>227471.52307940036</v>
+        <v>202427.2846191006</v>
       </c>
       <c r="AA16" s="11">
         <f t="shared" si="12"/>
-        <v>669347.5230794003</v>
+        <v>644303.28461910062</v>
       </c>
       <c r="AB16" s="11">
         <f t="shared" si="13"/>
@@ -18623,30 +18605,30 @@
       </c>
       <c r="AC16" s="12">
         <f t="shared" si="14"/>
-        <v>42738.536985777035</v>
+        <v>36143.606258885731</v>
       </c>
       <c r="AD16" s="12">
         <f t="shared" si="15"/>
-        <v>68030.977299367383</v>
+        <v>61436.04657247608</v>
       </c>
       <c r="AE16" s="12">
         <f t="shared" si="16"/>
-        <v>197318.19656351471</v>
+        <v>190723.26583662344</v>
       </c>
       <c r="AF16" s="12">
         <f t="shared" si="17"/>
-        <v>37135.901219160878</v>
+        <v>30540.970492269582</v>
       </c>
       <c r="AG16" s="12">
         <f t="shared" si="18"/>
-        <v>59900.361491412863</v>
+        <v>53305.430764521559</v>
       </c>
       <c r="AH16" s="12">
         <f t="shared" si="19"/>
-        <v>176260.12281916614</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+        <v>169665.19209227487</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2033</v>
       </c>
@@ -18702,31 +18684,31 @@
       </c>
       <c r="U17" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V17" s="11">
         <f t="shared" si="8"/>
-        <v>221375.52307940036</v>
+        <v>196331.2846191006</v>
       </c>
       <c r="W17" s="11">
         <f t="shared" si="9"/>
-        <v>339587.52307940036</v>
+        <v>314543.28461910062</v>
       </c>
       <c r="X17" s="11">
         <f t="shared" si="1"/>
-        <v>749363.5230794003</v>
+        <v>724319.28461910062</v>
       </c>
       <c r="Y17" s="11">
         <f t="shared" si="10"/>
-        <v>194195.52307940036</v>
+        <v>169151.2846191006</v>
       </c>
       <c r="Z17" s="11">
         <f t="shared" si="11"/>
-        <v>300599.52307940036</v>
+        <v>275555.28461910062</v>
       </c>
       <c r="AA17" s="11">
         <f t="shared" si="12"/>
-        <v>669395.5230794003</v>
+        <v>644351.28461910062</v>
       </c>
       <c r="AB17" s="11">
         <f t="shared" si="13"/>
@@ -18734,30 +18716,30 @@
       </c>
       <c r="AC17" s="12">
         <f t="shared" si="14"/>
-        <v>52995.540150148183</v>
+        <v>47000.148580246998</v>
       </c>
       <c r="AD17" s="12">
         <f t="shared" si="15"/>
-        <v>81294.553090175716</v>
+        <v>75299.161520274545</v>
       </c>
       <c r="AE17" s="12">
         <f t="shared" si="16"/>
-        <v>179391.66951247401</v>
+        <v>173396.27794257284</v>
       </c>
       <c r="AF17" s="12">
         <f t="shared" si="17"/>
-        <v>46488.864248294318</v>
+        <v>40493.47267839314</v>
       </c>
       <c r="AG17" s="12">
         <f t="shared" si="18"/>
-        <v>71961.135869370773</v>
+        <v>65965.744299469603</v>
       </c>
       <c r="AH17" s="12">
         <f t="shared" si="19"/>
-        <v>160247.96610852075</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+        <v>154252.57453861958</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2034</v>
       </c>
@@ -18813,31 +18795,31 @@
       </c>
       <c r="U18" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V18" s="11">
         <f t="shared" si="8"/>
-        <v>289331.52307940036</v>
+        <v>264287.28461910062</v>
       </c>
       <c r="W18" s="11">
         <f t="shared" si="9"/>
-        <v>425243.52307940036</v>
+        <v>400199.28461910062</v>
       </c>
       <c r="X18" s="11">
         <f t="shared" si="1"/>
-        <v>749387.5230794003</v>
+        <v>724343.28461910062</v>
       </c>
       <c r="Y18" s="11">
         <f t="shared" si="10"/>
-        <v>255359.52307940036</v>
+        <v>230315.2846191006</v>
       </c>
       <c r="Z18" s="11">
         <f t="shared" si="11"/>
-        <v>377699.52307940036</v>
+        <v>352655.28461910062</v>
       </c>
       <c r="AA18" s="11">
         <f t="shared" si="12"/>
-        <v>669407.5230794003</v>
+        <v>644363.28461910062</v>
       </c>
       <c r="AB18" s="11">
         <f t="shared" si="13"/>
@@ -18845,30 +18827,30 @@
       </c>
       <c r="AC18" s="12">
         <f t="shared" si="14"/>
-        <v>62966.969324617312</v>
+        <v>57516.613351979882</v>
       </c>
       <c r="AD18" s="12">
         <f t="shared" si="15"/>
-        <v>92545.380428127988</v>
+        <v>87095.024455490551</v>
       </c>
       <c r="AE18" s="12">
         <f t="shared" si="16"/>
-        <v>163088.55901968988</v>
+        <v>157638.20304705246</v>
       </c>
       <c r="AF18" s="12">
         <f t="shared" si="17"/>
-        <v>55573.67232355439</v>
+        <v>50123.316350916954</v>
       </c>
       <c r="AG18" s="12">
         <f t="shared" si="18"/>
-        <v>82198.420796121165</v>
+        <v>76748.064823483728</v>
       </c>
       <c r="AH18" s="12">
         <f t="shared" si="19"/>
-        <v>145682.5807391938</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+        <v>140232.22476655638</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2035</v>
       </c>
@@ -18915,31 +18897,31 @@
       </c>
       <c r="U19" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V19" s="11">
         <f t="shared" si="8"/>
-        <v>363383.52307940036</v>
+        <v>338339.28461910062</v>
       </c>
       <c r="W19" s="11">
         <f t="shared" si="9"/>
-        <v>507899.52307940036</v>
+        <v>482855.28461910062</v>
       </c>
       <c r="X19" s="11">
         <f t="shared" si="1"/>
-        <v>749399.5230794003</v>
+        <v>724355.28461910062</v>
       </c>
       <c r="Y19" s="11">
         <f t="shared" si="10"/>
-        <v>321995.52307940036</v>
+        <v>296951.28461910062</v>
       </c>
       <c r="Z19" s="11">
         <f t="shared" si="11"/>
-        <v>452075.52307940036</v>
+        <v>427031.28461910062</v>
       </c>
       <c r="AA19" s="11">
         <f t="shared" si="12"/>
-        <v>669419.5230794003</v>
+        <v>644375.28461910062</v>
       </c>
       <c r="AB19" s="11">
         <f t="shared" si="13"/>
@@ -18947,30 +18929,30 @@
       </c>
       <c r="AC19" s="12">
         <f t="shared" si="14"/>
-        <v>71893.492807408533</v>
+        <v>66938.623741374511</v>
       </c>
       <c r="AD19" s="12">
         <f t="shared" si="15"/>
-        <v>100485.21297818045</v>
+        <v>95530.343912146418</v>
       </c>
       <c r="AE19" s="12">
         <f t="shared" si="16"/>
-        <v>148264.70051756303</v>
+        <v>143309.83145152903</v>
       </c>
       <c r="AF19" s="12">
         <f t="shared" si="17"/>
-        <v>63705.09765096975</v>
+        <v>58750.228584935721</v>
       </c>
       <c r="AG19" s="12">
         <f t="shared" si="18"/>
-        <v>89440.732181499319</v>
+        <v>84485.863115465283</v>
       </c>
       <c r="AH19" s="12">
         <f t="shared" si="19"/>
-        <v>132441.08389893026</v>
-      </c>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+        <v>127486.21483289624</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2036</v>
       </c>
@@ -19017,31 +18999,31 @@
       </c>
       <c r="U20" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V20" s="11">
         <f t="shared" si="8"/>
-        <v>439019.52307940036</v>
+        <v>413975.28461910062</v>
       </c>
       <c r="W20" s="11">
         <f t="shared" si="9"/>
-        <v>580187.5230794003</v>
+        <v>555143.28461910062</v>
       </c>
       <c r="X20" s="11">
         <f t="shared" si="1"/>
-        <v>749447.5230794003</v>
+        <v>724403.28461910062</v>
       </c>
       <c r="Y20" s="11">
         <f t="shared" si="10"/>
-        <v>390095.52307940036</v>
+        <v>365051.28461910062</v>
       </c>
       <c r="Z20" s="11">
         <f t="shared" si="11"/>
-        <v>517127.52307940036</v>
+        <v>492083.28461910062</v>
       </c>
       <c r="AA20" s="11">
         <f t="shared" si="12"/>
-        <v>669467.5230794003</v>
+        <v>644423.28461910062</v>
       </c>
       <c r="AB20" s="11">
         <f t="shared" si="13"/>
@@ -19049,30 +19031,30 @@
       </c>
       <c r="AC20" s="12">
         <f t="shared" si="14"/>
-        <v>78961.520167581039</v>
+        <v>74457.093743913734</v>
       </c>
       <c r="AD20" s="12">
         <f t="shared" si="15"/>
-        <v>104351.8258214849</v>
+        <v>99847.399397817615</v>
       </c>
       <c r="AE20" s="12">
         <f t="shared" si="16"/>
-        <v>134794.72460151839</v>
+        <v>130290.29817785112</v>
       </c>
       <c r="AF20" s="12">
         <f t="shared" si="17"/>
-        <v>70162.108730062668</v>
+        <v>65657.682306395378</v>
       </c>
       <c r="AG20" s="12">
         <f t="shared" si="18"/>
-        <v>93009.930529809892</v>
+        <v>88505.504106142602</v>
       </c>
       <c r="AH20" s="12">
         <f t="shared" si="19"/>
-        <v>120409.6185845795</v>
-      </c>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+        <v>115905.19216091221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2037</v>
       </c>
@@ -19119,31 +19101,31 @@
       </c>
       <c r="U21" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V21" s="11">
         <f t="shared" si="8"/>
-        <v>510983.52307940036</v>
+        <v>485939.28461910062</v>
       </c>
       <c r="W21" s="11">
         <f t="shared" si="9"/>
-        <v>637415.5230794003</v>
+        <v>612371.28461910062</v>
       </c>
       <c r="X21" s="11">
         <f t="shared" si="1"/>
-        <v>749459.5230794003</v>
+        <v>724415.28461910062</v>
       </c>
       <c r="Y21" s="11">
         <f t="shared" si="10"/>
-        <v>454847.52307940036</v>
+        <v>429803.28461910062</v>
       </c>
       <c r="Z21" s="11">
         <f t="shared" si="11"/>
-        <v>568631.5230794003</v>
+        <v>543587.28461910062</v>
       </c>
       <c r="AA21" s="11">
         <f t="shared" si="12"/>
-        <v>669479.5230794003</v>
+        <v>644435.28461910062</v>
       </c>
       <c r="AB21" s="11">
         <f t="shared" si="13"/>
@@ -19151,30 +19133,30 @@
       </c>
       <c r="AC21" s="12">
         <f t="shared" si="14"/>
-        <v>83549.889204188788</v>
+        <v>79454.956091763976</v>
       </c>
       <c r="AD21" s="12">
         <f t="shared" si="15"/>
-        <v>104222.53150037213</v>
+        <v>100127.59838794734</v>
       </c>
       <c r="AE21" s="12">
         <f t="shared" si="16"/>
-        <v>122542.62082454297</v>
+        <v>118447.68771211818</v>
       </c>
       <c r="AF21" s="12">
         <f t="shared" si="17"/>
-        <v>74371.204631149143</v>
+        <v>70276.271518724316</v>
       </c>
       <c r="AG21" s="12">
         <f t="shared" si="18"/>
-        <v>92975.797859358179</v>
+        <v>88880.864746933381</v>
       </c>
       <c r="AH21" s="12">
         <f t="shared" si="19"/>
-        <v>109465.25171823488</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
+        <v>105370.31860581008</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2038</v>
       </c>
@@ -19221,31 +19203,31 @@
       </c>
       <c r="U22" s="7">
         <f>OPEX!$B$15</f>
-        <v>50088.476920599649</v>
+        <v>75132.715380899404</v>
       </c>
       <c r="V22" s="11">
         <f t="shared" si="8"/>
-        <v>574415.5230794003</v>
+        <v>549371.28461910062</v>
       </c>
       <c r="W22" s="11">
         <f t="shared" si="9"/>
-        <v>678731.5230794003</v>
+        <v>653687.28461910062</v>
       </c>
       <c r="X22" s="11">
         <f t="shared" si="1"/>
-        <v>749459.5230794003</v>
+        <v>724415.28461910062</v>
       </c>
       <c r="Y22" s="11">
         <f t="shared" si="10"/>
-        <v>511943.52307940036</v>
+        <v>486899.28461910062</v>
       </c>
       <c r="Z22" s="11">
         <f t="shared" si="11"/>
-        <v>605831.5230794003</v>
+        <v>580787.28461910062</v>
       </c>
       <c r="AA22" s="11">
         <f t="shared" si="12"/>
-        <v>669479.5230794003</v>
+        <v>644435.28461910062</v>
       </c>
       <c r="AB22" s="11">
         <f t="shared" si="13"/>
@@ -19253,30 +19235,30 @@
       </c>
       <c r="AC22" s="12">
         <f t="shared" si="14"/>
-        <v>85383.207343908187</v>
+        <v>81660.540878067462</v>
       </c>
       <c r="AD22" s="12">
         <f t="shared" si="15"/>
-        <v>100889.11604487474</v>
+        <v>97166.449579034015</v>
       </c>
       <c r="AE22" s="12">
         <f t="shared" si="16"/>
-        <v>111402.38256776637</v>
+        <v>107679.71610192563</v>
       </c>
       <c r="AF22" s="12">
         <f t="shared" si="17"/>
-        <v>76097.142613983902</v>
+        <v>72374.476148143163</v>
       </c>
       <c r="AG22" s="12">
         <f t="shared" si="18"/>
-        <v>90052.995561914679</v>
+        <v>86330.329096073954</v>
       </c>
       <c r="AH22" s="12">
         <f t="shared" si="19"/>
-        <v>99513.86519839536</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
+        <v>95791.198732554636</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="J25" s="3">
         <v>62974</v>
       </c>
@@ -19287,7 +19269,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -19295,7 +19277,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -19318,7 +19300,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2018</v>
       </c>
@@ -19353,7 +19335,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2019</v>
       </c>
@@ -19388,7 +19370,7 @@
         <v>6361</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2020</v>
       </c>
@@ -19417,7 +19399,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2021</v>
       </c>
@@ -19446,7 +19428,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2022</v>
       </c>
@@ -19475,7 +19457,7 @@
         <v>2486</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -19504,7 +19486,7 @@
         <v>4790</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2024</v>
       </c>
@@ -19547,7 +19529,7 @@
       <c r="AC35" s="10"/>
       <c r="AD35" s="10"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2025</v>
       </c>
@@ -19576,7 +19558,7 @@
         <v>16218</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2026</v>
       </c>
@@ -19605,7 +19587,7 @@
         <v>26652</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2027</v>
       </c>
@@ -19634,7 +19616,7 @@
         <v>37801</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2028</v>
       </c>
@@ -19663,7 +19645,7 @@
         <v>44496</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2029</v>
       </c>
@@ -19692,7 +19674,7 @@
         <v>45930</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2030</v>
       </c>
@@ -19721,7 +19703,7 @@
         <v>45996</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2031</v>
       </c>
@@ -19750,7 +19732,7 @@
         <v>46006</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2032</v>
       </c>
@@ -19779,7 +19761,7 @@
         <v>46012</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2033</v>
       </c>
@@ -19808,7 +19790,7 @@
         <v>46016</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2034</v>
       </c>
@@ -19837,7 +19819,7 @@
         <v>46017</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2035</v>
       </c>
@@ -19866,7 +19848,7 @@
         <v>46018</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2036</v>
       </c>
@@ -19895,7 +19877,7 @@
         <v>46019</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2037</v>
       </c>
@@ -19924,7 +19906,7 @@
         <v>46020</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2038</v>
       </c>
@@ -19953,12 +19935,12 @@
         <v>46020</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -19981,7 +19963,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2018</v>
       </c>
@@ -20010,7 +19992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2019</v>
       </c>
@@ -20039,7 +20021,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>2020</v>
       </c>
@@ -20068,7 +20050,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>2021</v>
       </c>
@@ -20097,7 +20079,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>2022</v>
       </c>
@@ -20126,7 +20108,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -20155,7 +20137,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>2024</v>
       </c>
@@ -20184,7 +20166,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>2025</v>
       </c>
@@ -20213,7 +20195,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>2026</v>
       </c>
@@ -20242,7 +20224,7 @@
         <v>2691</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>2027</v>
       </c>
@@ -20271,7 +20253,7 @@
         <v>3817</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>2028</v>
       </c>
@@ -20300,7 +20282,7 @@
         <v>4493</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>2029</v>
       </c>
@@ -20329,7 +20311,7 @@
         <v>4638</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>2030</v>
       </c>
@@ -20358,7 +20340,7 @@
         <v>4645</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>2031</v>
       </c>
@@ -20387,7 +20369,7 @@
         <v>4646</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>2032</v>
       </c>
@@ -20416,7 +20398,7 @@
         <v>4647</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2033</v>
       </c>
@@ -20445,7 +20427,7 @@
         <v>4647</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>2034</v>
       </c>
@@ -20474,7 +20456,7 @@
         <v>4647</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>2035</v>
       </c>
@@ -20503,7 +20485,7 @@
         <v>4647</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>2036</v>
       </c>
@@ -20532,7 +20514,7 @@
         <v>4648</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>2037</v>
       </c>
@@ -20561,7 +20543,7 @@
         <v>4648</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>2038</v>
       </c>
@@ -20608,9 +20590,9 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="14.88671875" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -22060,7 +22042,7 @@
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -23509,7 +23491,7 @@
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -24958,7 +24940,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -26407,7 +26389,7 @@
       <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -27856,7 +27838,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Commit after generating final results. Comments and code cleaning underway
</commit_message>
<xml_diff>
--- a/tumlknexpectimax/excel_data/input_data_NY_business.xlsx
+++ b/tumlknexpectimax/excel_data/input_data_NY_business.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="705" windowWidth="13680" windowHeight="11190" tabRatio="847" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="765" windowWidth="13680" windowHeight="11130" tabRatio="847" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
@@ -899,10 +899,10 @@
                   <c:v>123966.4385182156</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>148601.5257512136</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>162896.27914347179</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>148601.5257512136</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>148601.5257512136</c:v>
@@ -911,7 +911,7 @@
                   <c:v>148601.5257512136</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>148601.5257512136</c:v>
+                  <c:v>162896.27914347179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1107,43 +1107,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>3198.8888888888887</c:v>
+                  <c:v>3419.7777777777778</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7420</c:v>
+                  <c:v>7900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6458</c:v>
+                  <c:v>7232.1111111111113</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7164</c:v>
+                  <c:v>8289</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29050</c:v>
+                  <c:v>30450</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7690</c:v>
+                  <c:v>19660.666666666668</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14840</c:v>
+                  <c:v>17040</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13828</c:v>
+                  <c:v>15506</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4920</c:v>
+                  <c:v>5360</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10700</c:v>
+                  <c:v>12380</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21000</c:v>
+                  <c:v>24400</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34480</c:v>
+                  <c:v>38000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21000</c:v>
+                  <c:v>22000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1223,43 +1223,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>118366.39999999999</c:v>
+                  <c:v>119020.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100181.6</c:v>
+                  <c:v>116275.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96800</c:v>
+                  <c:v>98960</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>278720</c:v>
+                  <c:v>341360</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>262692.8</c:v>
+                  <c:v>327450</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>148579.6</c:v>
+                  <c:v>166336.79999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>61989.9</c:v>
+                  <c:v>195632.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>200640</c:v>
+                  <c:v>201120</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>78450.2</c:v>
+                  <c:v>79394</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89988.6</c:v>
+                  <c:v>89994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>355977.2</c:v>
+                  <c:v>228180</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>260532.4</c:v>
+                  <c:v>272276</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>215177.2</c:v>
+                  <c:v>215380</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1280,11 +1280,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="61426176"/>
-        <c:axId val="60879936"/>
+        <c:axId val="245663232"/>
+        <c:axId val="233240768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61426176"/>
+        <c:axId val="245663232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,7 +1313,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60879936"/>
+        <c:crossAx val="233240768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1321,7 +1321,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60879936"/>
+        <c:axId val="233240768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1351,7 +1351,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61426176"/>
+        <c:crossAx val="245663232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1485,46 +1485,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>54093.51440637085</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28924.563178455599</c:v>
+                  <c:v>42365.673348618162</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65564.735538328358</c:v>
+                  <c:v>42358.112806224512</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66372.633078806393</c:v>
+                  <c:v>42902.769000487555</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15811.164779648698</c:v>
+                  <c:v>35408.524500181637</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17908.3780335597</c:v>
+                  <c:v>40576.763975644033</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>76475.574182744094</c:v>
+                  <c:v>37982.807078103164</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>71590.2951000045</c:v>
+                  <c:v>43544.075083463555</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72330.433753814403</c:v>
+                  <c:v>45178.949649365633</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56524.301570279997</c:v>
+                  <c:v>22360.217706464937</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>67241.808150316792</c:v>
+                  <c:v>24572.597341958404</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18209.722395299548</c:v>
+                  <c:v>43083.217137892461</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>71129.362140663448</c:v>
+                  <c:v>52368.522953392559</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>75132.715380899404</c:v>
+                  <c:v>49441.019044068453</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1544,11 +1544,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="61519360"/>
-        <c:axId val="60882240"/>
+        <c:axId val="242300928"/>
+        <c:axId val="246063680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61519360"/>
+        <c:axId val="242300928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,7 +1558,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60882240"/>
+        <c:crossAx val="246063680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1566,7 +1566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60882240"/>
+        <c:axId val="246063680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1596,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61519360"/>
+        <c:crossAx val="242300928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1925,11 +1925,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="63198720"/>
-        <c:axId val="61383808"/>
+        <c:axId val="246485504"/>
+        <c:axId val="246065408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="63198720"/>
+        <c:axId val="246485504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,7 +1949,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61383808"/>
+        <c:crossAx val="246065408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1957,7 +1957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61383808"/>
+        <c:axId val="246065408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1980,7 +1980,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1997,7 +1996,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63198720"/>
+        <c:crossAx val="246485504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2579,11 +2578,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="63072768"/>
-        <c:axId val="61386112"/>
+        <c:axId val="246814208"/>
+        <c:axId val="246067712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="63072768"/>
+        <c:axId val="246814208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2593,7 +2592,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61386112"/>
+        <c:crossAx val="246067712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2601,7 +2600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61386112"/>
+        <c:axId val="246067712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2612,7 +2611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63072768"/>
+        <c:crossAx val="246814208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2653,7 +2652,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2694,7 +2693,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2735,7 +2734,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2776,7 +2775,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3087,7 +3086,7 @@
   <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:V15"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3220,11 +3219,13 @@
       <c r="U2" s="13"/>
       <c r="V2" s="13"/>
       <c r="W2" s="13">
-        <v>10000</v>
-      </c>
-      <c r="X2" s="13"/>
-    </row>
-    <row r="3" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>100000</v>
+      </c>
+      <c r="X2" s="13">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>73</v>
       </c>
@@ -3290,21 +3291,21 @@
         <v>35.517736249908381</v>
       </c>
       <c r="U3" s="11">
-        <v>3198.8888888888887</v>
+        <v>3419.7777777777778</v>
       </c>
       <c r="V3" s="11">
-        <v>118366.39999999999</v>
+        <v>119020.4</v>
       </c>
       <c r="W3" s="11">
         <f>SUM(U3,V3)</f>
-        <v>121565.28888888888</v>
+        <v>122440.17777777778</v>
       </c>
       <c r="X3" s="12">
         <f t="shared" ref="X3:X14" si="0">S3+T3+U3+V3</f>
-        <v>291788.63717996189</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>292663.52606885077</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>66</v>
       </c>
@@ -3370,21 +3371,21 @@
         <v>35.517736249908381</v>
       </c>
       <c r="U4" s="11">
-        <v>7420</v>
+        <v>7900</v>
       </c>
       <c r="V4" s="11">
-        <v>100181.6</v>
+        <v>116275.2</v>
       </c>
       <c r="W4" s="11">
         <f t="shared" ref="W4:W15" si="2">SUM(U4,V4)</f>
-        <v>107601.60000000001</v>
+        <v>124175.2</v>
       </c>
       <c r="X4" s="12">
         <f t="shared" si="0"/>
-        <v>277824.94829107303</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>294398.54829107301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>67</v>
       </c>
@@ -3446,21 +3447,21 @@
         <v>23.727612871311063</v>
       </c>
       <c r="U5" s="11">
-        <v>6458</v>
+        <v>7232.1111111111113</v>
       </c>
       <c r="V5" s="11">
-        <v>96800</v>
+        <v>98960</v>
       </c>
       <c r="W5" s="11">
         <f t="shared" si="2"/>
-        <v>103258</v>
+        <v>106192.11111111111</v>
       </c>
       <c r="X5" s="12">
         <f t="shared" si="0"/>
-        <v>227248.16613108691</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>230182.27724219803</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
@@ -3526,21 +3527,21 @@
         <v>23.727612871311063</v>
       </c>
       <c r="U6" s="11">
-        <v>7164</v>
+        <v>8289</v>
       </c>
       <c r="V6" s="11">
-        <v>278720</v>
+        <v>341360</v>
       </c>
       <c r="W6" s="11">
         <f t="shared" si="2"/>
-        <v>285884</v>
+        <v>349649</v>
       </c>
       <c r="X6" s="12">
         <f t="shared" si="0"/>
-        <v>409874.16613108688</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>473639.16613108688</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>69</v>
       </c>
@@ -3606,21 +3607,21 @@
         <v>35.517736249908381</v>
       </c>
       <c r="U7" s="11">
-        <v>29050</v>
+        <v>30450</v>
       </c>
       <c r="V7" s="11">
-        <v>262692.8</v>
+        <v>327450</v>
       </c>
       <c r="W7" s="11">
         <f t="shared" si="2"/>
-        <v>291742.8</v>
+        <v>357900</v>
       </c>
       <c r="X7" s="12">
         <f t="shared" si="0"/>
-        <v>461966.14829107304</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>528123.34829107299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>70</v>
       </c>
@@ -3684,21 +3685,21 @@
         <v>35.517736249908381</v>
       </c>
       <c r="U8" s="11">
-        <v>7690</v>
+        <v>19660.666666666668</v>
       </c>
       <c r="V8" s="11">
-        <v>148579.6</v>
+        <v>166336.79999999999</v>
       </c>
       <c r="W8" s="11">
         <f t="shared" si="2"/>
-        <v>156269.6</v>
+        <v>185997.46666666665</v>
       </c>
       <c r="X8" s="12">
         <f t="shared" si="0"/>
-        <v>326492.94829107303</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>356220.81495773967</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>71</v>
       </c>
@@ -3762,21 +3763,21 @@
         <v>35.517736249908381</v>
       </c>
       <c r="U9" s="11">
-        <v>14840</v>
+        <v>17040</v>
       </c>
       <c r="V9" s="11">
-        <v>61989.9</v>
+        <v>195632.2</v>
       </c>
       <c r="W9" s="11">
         <f t="shared" si="2"/>
-        <v>76829.899999999994</v>
+        <v>212672.2</v>
       </c>
       <c r="X9" s="12">
         <f t="shared" si="0"/>
-        <v>247053.24829107302</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>382895.54829107306</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>72</v>
       </c>
@@ -3839,21 +3840,21 @@
         <v>23.727612871311063</v>
       </c>
       <c r="U10" s="11">
-        <v>13828</v>
+        <v>15506</v>
       </c>
       <c r="V10" s="11">
-        <v>200640</v>
+        <v>201120</v>
       </c>
       <c r="W10" s="11">
         <f t="shared" si="2"/>
-        <v>214468</v>
+        <v>216626</v>
       </c>
       <c r="X10" s="12">
         <f t="shared" si="0"/>
-        <v>338458.16613108688</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>340616.16613108688</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
@@ -3911,27 +3912,27 @@
         <v>1544140.8019904599</v>
       </c>
       <c r="S11" s="11">
-        <v>162896.27914347179</v>
+        <v>148601.5257512136</v>
       </c>
       <c r="T11" s="11">
         <v>33.851521342501684</v>
       </c>
       <c r="U11" s="11">
-        <v>4920</v>
+        <v>5360</v>
       </c>
       <c r="V11" s="11">
-        <v>78450.2</v>
+        <v>79394</v>
       </c>
       <c r="W11" s="11">
         <f t="shared" si="2"/>
-        <v>83370.2</v>
+        <v>84754</v>
       </c>
       <c r="X11" s="12">
         <f t="shared" si="0"/>
-        <v>246300.33066481428</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>233389.3772725561</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>75</v>
       </c>
@@ -3989,27 +3990,27 @@
         <v>1544140.8019904599</v>
       </c>
       <c r="S12" s="11">
-        <v>148601.5257512136</v>
+        <v>162896.27914347179</v>
       </c>
       <c r="T12" s="11">
         <v>33.851521342501684</v>
       </c>
       <c r="U12" s="11">
-        <v>10700</v>
+        <v>12380</v>
       </c>
       <c r="V12" s="11">
-        <v>89988.6</v>
+        <v>89994</v>
       </c>
       <c r="W12" s="11">
         <f t="shared" si="2"/>
-        <v>100688.6</v>
+        <v>102374</v>
       </c>
       <c r="X12" s="12">
         <f t="shared" si="0"/>
-        <v>249323.97727255611</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>265304.13066481426</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
@@ -4073,21 +4074,21 @@
         <v>33.851521342501684</v>
       </c>
       <c r="U13" s="11">
-        <v>21000</v>
+        <v>24400</v>
       </c>
       <c r="V13" s="11">
-        <v>355977.2</v>
+        <v>228180</v>
       </c>
       <c r="W13" s="11">
         <f t="shared" si="2"/>
-        <v>376977.2</v>
+        <v>252580</v>
       </c>
       <c r="X13" s="12">
         <f t="shared" si="0"/>
-        <v>525612.57727255614</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>401215.37727255607</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>77</v>
       </c>
@@ -4151,21 +4152,21 @@
         <v>33.851521342501684</v>
       </c>
       <c r="U14" s="11">
-        <v>34480</v>
+        <v>38000</v>
       </c>
       <c r="V14" s="11">
-        <v>260532.4</v>
+        <v>272276</v>
       </c>
       <c r="W14" s="11">
         <f t="shared" si="2"/>
-        <v>295012.40000000002</v>
+        <v>310276</v>
       </c>
       <c r="X14" s="12">
         <f t="shared" si="0"/>
-        <v>443647.77727255609</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>458911.37727255607</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>78</v>
       </c>
@@ -4223,24 +4224,24 @@
         <v>1544140.8019904599</v>
       </c>
       <c r="S15" s="11">
-        <v>148601.5257512136</v>
+        <v>162896.27914347179</v>
       </c>
       <c r="T15" s="11">
         <v>33.851521342501684</v>
       </c>
       <c r="U15" s="11">
-        <v>21000</v>
+        <v>22000</v>
       </c>
       <c r="V15" s="11">
-        <v>215177.2</v>
+        <v>215380</v>
       </c>
       <c r="W15" s="11">
         <f t="shared" si="2"/>
-        <v>236177.2</v>
+        <v>237380</v>
       </c>
       <c r="X15" s="12">
         <f t="shared" ref="X15" si="5">SUM(S15:V15)</f>
-        <v>384812.57727255614</v>
+        <v>400310.13066481426</v>
       </c>
     </row>
     <row r="27" spans="17:17" ht="14.45" x14ac:dyDescent="0.3">
@@ -4249,7 +4250,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="42" spans="18:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R42" s="5" t="s">
         <v>52</v>
       </c>
@@ -4263,12 +4264,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="18:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="18:25" x14ac:dyDescent="0.25">
       <c r="S43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="18:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R44" t="s">
         <v>55</v>
       </c>
@@ -4288,7 +4289,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="18:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="18:25" x14ac:dyDescent="0.25">
       <c r="S45" t="s">
         <v>57</v>
       </c>
@@ -4299,7 +4300,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="18:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R46" t="s">
         <v>60</v>
       </c>
@@ -16005,55 +16006,55 @@
       </c>
       <c r="C2">
         <f>CAPEX!$X3</f>
-        <v>291788.63717996189</v>
+        <v>292663.52606885077</v>
       </c>
       <c r="D2">
         <f>CAPEX!$X4</f>
-        <v>277824.94829107303</v>
+        <v>294398.54829107301</v>
       </c>
       <c r="E2">
         <f>CAPEX!$X5</f>
-        <v>227248.16613108691</v>
+        <v>230182.27724219803</v>
       </c>
       <c r="F2">
         <f>CAPEX!$X6</f>
-        <v>409874.16613108688</v>
+        <v>473639.16613108688</v>
       </c>
       <c r="G2">
         <f>CAPEX!$X7</f>
-        <v>461966.14829107304</v>
+        <v>528123.34829107299</v>
       </c>
       <c r="H2">
         <f>CAPEX!$X8</f>
-        <v>326492.94829107303</v>
+        <v>356220.81495773967</v>
       </c>
       <c r="I2">
         <f>CAPEX!$X9</f>
-        <v>247053.24829107302</v>
+        <v>382895.54829107306</v>
       </c>
       <c r="J2">
         <f>CAPEX!$X10</f>
-        <v>338458.16613108688</v>
+        <v>340616.16613108688</v>
       </c>
       <c r="K2">
         <f>CAPEX!$X11</f>
-        <v>246300.33066481428</v>
+        <v>233389.3772725561</v>
       </c>
       <c r="L2">
         <f>CAPEX!$X12</f>
-        <v>249323.97727255611</v>
+        <v>265304.13066481426</v>
       </c>
       <c r="M2">
         <f>CAPEX!$X13</f>
-        <v>525612.57727255614</v>
+        <v>401215.37727255607</v>
       </c>
       <c r="N2">
         <f>CAPEX!$X14</f>
-        <v>443647.77727255609</v>
+        <v>458911.37727255607</v>
       </c>
       <c r="O2">
         <f>CAPEX!$X15</f>
-        <v>384812.57727255614</v>
+        <v>400310.13066481426</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -16068,7 +16069,7 @@
       </c>
       <c r="D3">
         <f>D2-C2</f>
-        <v>-13963.688888888864</v>
+        <v>1735.0222222222365</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -16078,15 +16079,15 @@
       </c>
       <c r="G3">
         <f>G2-C2</f>
-        <v>170177.51111111115</v>
+        <v>235459.82222222222</v>
       </c>
       <c r="H3">
         <f>H2-C2</f>
-        <v>34704.311111111136</v>
+        <v>63557.288888888899</v>
       </c>
       <c r="I3">
         <f>I2-D2+D3</f>
-        <v>-44735.388888888876</v>
+        <v>90232.022222222295</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -16128,14 +16129,14 @@
       </c>
       <c r="G4">
         <f>G2-D2</f>
-        <v>184141.2</v>
+        <v>233724.79999999999</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
         <f>I2-D2</f>
-        <v>-30771.700000000012</v>
+        <v>88497.000000000058</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -16174,7 +16175,7 @@
       </c>
       <c r="F5">
         <f>F2-E2</f>
-        <v>182625.99999999997</v>
+        <v>243456.88888888885</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -16187,7 +16188,7 @@
       </c>
       <c r="J5">
         <f>J2-E2</f>
-        <v>111209.99999999997</v>
+        <v>110433.88888888885</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -16320,14 +16321,14 @@
       </c>
       <c r="G8">
         <f>G2-H2</f>
-        <v>135473.20000000001</v>
+        <v>171902.53333333333</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
         <f>I2-H2</f>
-        <v>-79439.700000000012</v>
+        <v>26674.733333333395</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -16369,7 +16370,7 @@
       </c>
       <c r="G9">
         <f>G2-I2</f>
-        <v>214912.90000000002</v>
+        <v>145227.79999999993</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -16414,7 +16415,7 @@
       </c>
       <c r="F10">
         <f>F2-J2</f>
-        <v>71416</v>
+        <v>133023</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -16480,19 +16481,19 @@
       </c>
       <c r="L11">
         <f>L2-K2</f>
-        <v>3023.6466077418299</v>
+        <v>31914.753392258164</v>
       </c>
       <c r="M11">
         <f>M2-K2</f>
-        <v>279312.24660774186</v>
+        <v>167825.99999999997</v>
       </c>
       <c r="N11">
         <f>N2-K2</f>
-        <v>197347.44660774182</v>
+        <v>225521.99999999997</v>
       </c>
       <c r="O11">
         <f>O2-L2+L11</f>
-        <v>138512.24660774186</v>
+        <v>166920.75339225816</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -16534,14 +16535,14 @@
       </c>
       <c r="M12">
         <f>M2-L2</f>
-        <v>276288.60000000003</v>
+        <v>135911.24660774181</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
         <f>O2-L2</f>
-        <v>135488.60000000003</v>
+        <v>135006</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -16630,14 +16631,14 @@
       </c>
       <c r="M14">
         <f>M2-N2</f>
-        <v>81964.800000000047</v>
+        <v>-57696</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
         <f>O2-N2</f>
-        <v>-58835.199999999953</v>
+        <v>-58601.246607741807</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -16679,7 +16680,7 @@
       </c>
       <c r="M15">
         <f>M2-O2</f>
-        <v>140800</v>
+        <v>905.24660774180666</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -16718,7 +16719,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16741,125 +16742,111 @@
         <v>23</v>
       </c>
       <c r="B2" s="12">
-        <f>AVERAGE(B3:B15)</f>
-        <v>54093.51440637085</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>73</v>
       </c>
       <c r="B3" s="12">
-        <f>1.5*19283.0421189704</f>
-        <v>28924.563178455599</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>42365.673348618162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B4" s="12">
-        <f>1.5*43709.8236922189</f>
-        <v>65564.735538328358</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>42358.112806224512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B5" s="12">
-        <f>1.5*44248.4220525376</f>
-        <v>66372.633078806393</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>42902.769000487555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
       <c r="B6" s="12">
-        <f>1.5*10540.7765197658</f>
-        <v>15811.164779648698</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>35408.524500181637</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="12">
-        <f>1.5*11938.9186890398</f>
-        <v>17908.3780335597</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>40576.763975644033</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="12">
-        <f>1.5*50983.7161218294</f>
-        <v>76475.574182744094</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37982.807078103164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="12">
-        <f>1.5*47726.863400003</f>
-        <v>71590.2951000045</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>43544.075083463555</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>72</v>
       </c>
       <c r="B10" s="12">
-        <f>1.5*48220.2891692096</f>
-        <v>72330.433753814403</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>45178.949649365633</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
       <c r="B11" s="12">
-        <f>1.5*37682.86771352</f>
-        <v>56524.301570279997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>22360.217706464937</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B12" s="12">
-        <f>1.5*44827.8721002112</f>
-        <v>67241.808150316792</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>24572.597341958404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B13" s="12">
-        <f>1.5*12139.8149301997</f>
-        <v>18209.722395299548</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>43083.217137892461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B14" s="12">
-        <f>1.5*47419.5747604423</f>
-        <v>71129.362140663448</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>52368.522953392559</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>78</v>
       </c>
       <c r="B15" s="12">
-        <f>1.5*50088.4769205996</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
     </row>
   </sheetData>
@@ -17023,31 +17010,31 @@
       </c>
       <c r="U2" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V2" s="11">
         <f>O2-U2</f>
-        <v>-71880.715380899404</v>
+        <v>-46189.019044068453</v>
       </c>
       <c r="W2" s="11">
         <f>P2-U2</f>
-        <v>-71880.715380899404</v>
+        <v>-46189.019044068453</v>
       </c>
       <c r="X2" s="11">
         <f t="shared" ref="X2:X22" si="1">Q2-U2</f>
-        <v>-71880.715380899404</v>
+        <v>-46189.019044068453</v>
       </c>
       <c r="Y2" s="11">
         <f>R2-$U2</f>
-        <v>-72240.715380899404</v>
+        <v>-46549.019044068453</v>
       </c>
       <c r="Z2" s="11">
         <f>S2-$U2</f>
-        <v>-72240.715380899404</v>
+        <v>-46549.019044068453</v>
       </c>
       <c r="AA2" s="11">
         <f>T2-$U2</f>
-        <v>-72240.715380899404</v>
+        <v>-46549.019044068453</v>
       </c>
       <c r="AB2" s="11">
         <f>1/POWER(1+$L$25,N2-2018)</f>
@@ -17055,27 +17042,27 @@
       </c>
       <c r="AC2" s="12">
         <f>V2*AB2</f>
-        <v>-71880.715380899404</v>
+        <v>-46189.019044068453</v>
       </c>
       <c r="AD2" s="12">
         <f>W2*AB2</f>
-        <v>-71880.715380899404</v>
+        <v>-46189.019044068453</v>
       </c>
       <c r="AE2" s="12">
         <f>X2*AB2</f>
-        <v>-71880.715380899404</v>
+        <v>-46189.019044068453</v>
       </c>
       <c r="AF2" s="12">
         <f>Y2*$AB2</f>
-        <v>-72240.715380899404</v>
+        <v>-46549.019044068453</v>
       </c>
       <c r="AG2" s="12">
         <f>Z2*$AB2</f>
-        <v>-72240.715380899404</v>
+        <v>-46549.019044068453</v>
       </c>
       <c r="AH2" s="12">
         <f>AA2*$AB2</f>
-        <v>-72240.715380899404</v>
+        <v>-46549.019044068453</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -17125,31 +17112,31 @@
       </c>
       <c r="U3" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V3" s="11">
         <f t="shared" ref="V3:V22" si="8">O3-U3</f>
-        <v>-70860.715380899404</v>
+        <v>-45169.019044068453</v>
       </c>
       <c r="W3" s="11">
         <f t="shared" ref="W3:W22" si="9">P3-U3</f>
-        <v>-70716.715380899404</v>
+        <v>-45025.019044068453</v>
       </c>
       <c r="X3" s="11">
         <f t="shared" si="1"/>
-        <v>-69096.715380899404</v>
+        <v>-43405.019044068453</v>
       </c>
       <c r="Y3" s="11">
         <f t="shared" ref="Y3:Y22" si="10">R3-$U3</f>
-        <v>-71304.715380899404</v>
+        <v>-45613.019044068453</v>
       </c>
       <c r="Z3" s="11">
         <f t="shared" ref="Z3:Z22" si="11">S3-$U3</f>
-        <v>-71172.715380899404</v>
+        <v>-45481.019044068453</v>
       </c>
       <c r="AA3" s="11">
         <f t="shared" ref="AA3:AA22" si="12">T3-$U3</f>
-        <v>-69708.715380899404</v>
+        <v>-44017.019044068453</v>
       </c>
       <c r="AB3" s="11">
         <f t="shared" ref="AB3:AB22" si="13">1/POWER(1+$L$25,N3-2018)</f>
@@ -17157,27 +17144,27 @@
       </c>
       <c r="AC3" s="12">
         <f t="shared" ref="AC3:AC22" si="14">V3*AB3</f>
-        <v>-64418.832164454005</v>
+        <v>-41062.744585516775</v>
       </c>
       <c r="AD3" s="12">
         <f t="shared" ref="AD3:AD22" si="15">W3*AB3</f>
-        <v>-64287.923073544909</v>
+        <v>-40931.83549460768</v>
       </c>
       <c r="AE3" s="12">
         <f t="shared" ref="AE3:AE22" si="16">X3*AB3</f>
-        <v>-62815.195800817637</v>
+        <v>-39459.108221880408</v>
       </c>
       <c r="AF3" s="12">
         <f t="shared" ref="AF3:AF22" si="17">Y3*$AB3</f>
-        <v>-64822.468528090365</v>
+        <v>-41466.380949153136</v>
       </c>
       <c r="AG3" s="12">
         <f t="shared" ref="AG3:AG22" si="18">Z3*$AB3</f>
-        <v>-64702.468528090365</v>
+        <v>-41346.380949153136</v>
       </c>
       <c r="AH3" s="12">
         <f t="shared" ref="AH3:AH22" si="19">AA3*$AB3</f>
-        <v>-63371.559437181277</v>
+        <v>-40015.471858244047</v>
       </c>
     </row>
     <row r="4" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -17236,31 +17223,31 @@
       </c>
       <c r="U4" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V4" s="11">
         <f t="shared" si="8"/>
-        <v>-69360.715380899404</v>
+        <v>-43669.019044068453</v>
       </c>
       <c r="W4" s="11">
         <f t="shared" si="9"/>
-        <v>-68988.715380899404</v>
+        <v>-43297.019044068453</v>
       </c>
       <c r="X4" s="11">
         <f t="shared" si="1"/>
-        <v>-63624.715380899404</v>
+        <v>-37933.019044068453</v>
       </c>
       <c r="Y4" s="11">
         <f t="shared" si="10"/>
-        <v>-69948.715380899404</v>
+        <v>-44257.019044068453</v>
       </c>
       <c r="Z4" s="11">
         <f t="shared" si="11"/>
-        <v>-69612.715380899404</v>
+        <v>-43921.019044068453</v>
       </c>
       <c r="AA4" s="11">
         <f t="shared" si="12"/>
-        <v>-64800.715380899404</v>
+        <v>-39109.019044068453</v>
       </c>
       <c r="AB4" s="11">
         <f t="shared" si="13"/>
@@ -17268,27 +17255,27 @@
       </c>
       <c r="AC4" s="12">
         <f t="shared" si="14"/>
-        <v>-57322.905273470577</v>
+        <v>-36090.098383527642</v>
       </c>
       <c r="AD4" s="12">
         <f t="shared" si="15"/>
-        <v>-57015.467256941651</v>
+        <v>-35782.660366998716</v>
       </c>
       <c r="AE4" s="12">
         <f t="shared" si="16"/>
-        <v>-52582.409405701983</v>
+        <v>-31349.602515759048</v>
       </c>
       <c r="AF4" s="12">
         <f t="shared" si="17"/>
-        <v>-57808.855686693714</v>
+        <v>-36576.048796750787</v>
       </c>
       <c r="AG4" s="12">
         <f t="shared" si="18"/>
-        <v>-57531.169736280492</v>
+        <v>-36298.362846337557</v>
       </c>
       <c r="AH4" s="12">
         <f t="shared" si="19"/>
-        <v>-53554.310232148266</v>
+        <v>-32321.503342205331</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -17348,31 +17335,31 @@
       </c>
       <c r="U5" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V5" s="11">
         <f t="shared" si="8"/>
-        <v>-67308.715380899404</v>
+        <v>-41617.019044068453</v>
       </c>
       <c r="W5" s="11">
         <f t="shared" si="9"/>
-        <v>-66468.715380899404</v>
+        <v>-40777.019044068453</v>
       </c>
       <c r="X5" s="11">
         <f t="shared" si="1"/>
-        <v>-52896.715380899404</v>
+        <v>-27205.019044068453</v>
       </c>
       <c r="Y5" s="11">
         <f t="shared" si="10"/>
-        <v>-68100.715380899404</v>
+        <v>-42409.019044068453</v>
       </c>
       <c r="Z5" s="11">
         <f t="shared" si="11"/>
-        <v>-67356.715380899404</v>
+        <v>-41665.019044068453</v>
       </c>
       <c r="AA5" s="11">
         <f t="shared" si="12"/>
-        <v>-55152.715380899404</v>
+        <v>-29461.019044068453</v>
       </c>
       <c r="AB5" s="11">
         <f t="shared" si="13"/>
@@ -17380,27 +17367,27 @@
       </c>
       <c r="AC5" s="12">
         <f t="shared" si="14"/>
-        <v>-50570.034095341383</v>
+        <v>-31267.482377211451</v>
       </c>
       <c r="AD5" s="12">
         <f t="shared" si="15"/>
-        <v>-49938.929662584058</v>
+        <v>-30636.377944454125</v>
       </c>
       <c r="AE5" s="12">
         <f t="shared" si="16"/>
-        <v>-39742.085184747848</v>
+        <v>-20439.533466617915</v>
       </c>
       <c r="AF5" s="12">
         <f t="shared" si="17"/>
-        <v>-51165.075417655433</v>
+        <v>-31862.5236995255</v>
       </c>
       <c r="AG5" s="12">
         <f t="shared" si="18"/>
-        <v>-50606.097205784659</v>
+        <v>-31303.545487654726</v>
       </c>
       <c r="AH5" s="12">
         <f t="shared" si="19"/>
-        <v>-41437.05137558181</v>
+        <v>-22134.499657451874</v>
       </c>
     </row>
     <row r="6" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -17460,31 +17447,31 @@
       </c>
       <c r="U6" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V6" s="11">
         <f t="shared" si="8"/>
-        <v>-64428.715380899404</v>
+        <v>-38737.019044068453</v>
       </c>
       <c r="W6" s="11">
         <f t="shared" si="9"/>
-        <v>-62904.715380899404</v>
+        <v>-37213.019044068453</v>
       </c>
       <c r="X6" s="11">
         <f t="shared" si="1"/>
-        <v>-31932.715380899404</v>
+        <v>-6241.0190440684528</v>
       </c>
       <c r="Y6" s="11">
         <f t="shared" si="10"/>
-        <v>-65508.715380899404</v>
+        <v>-39817.019044068453</v>
       </c>
       <c r="Z6" s="11">
         <f t="shared" si="11"/>
-        <v>-64140.715380899404</v>
+        <v>-38449.019044068453</v>
       </c>
       <c r="AA6" s="11">
         <f t="shared" si="12"/>
-        <v>-36264.715380899404</v>
+        <v>-10573.019044068453</v>
       </c>
       <c r="AB6" s="11">
         <f t="shared" si="13"/>
@@ -17492,27 +17479,27 @@
       </c>
       <c r="AC6" s="12">
         <f t="shared" si="14"/>
-        <v>-44005.679517040771</v>
+        <v>-26457.905227831736</v>
       </c>
       <c r="AD6" s="12">
         <f t="shared" si="15"/>
-        <v>-42964.767011064403</v>
+        <v>-25416.992721855368</v>
       </c>
       <c r="AE6" s="12">
         <f t="shared" si="16"/>
-        <v>-21810.474271497435</v>
+        <v>-4262.6999822884036</v>
       </c>
       <c r="AF6" s="12">
         <f t="shared" si="17"/>
-        <v>-44743.334048835044</v>
+        <v>-27195.559759626012</v>
       </c>
       <c r="AG6" s="12">
         <f t="shared" si="18"/>
-        <v>-43808.97164189563</v>
+        <v>-26261.197352686595</v>
       </c>
       <c r="AH6" s="12">
         <f t="shared" si="19"/>
-        <v>-24769.288560138921</v>
+        <v>-7221.5142709298889</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -17572,31 +17559,31 @@
       </c>
       <c r="U7" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V7" s="11">
         <f t="shared" si="8"/>
-        <v>-60516.715380899404</v>
+        <v>-34825.019044068453</v>
       </c>
       <c r="W7" s="11">
         <f t="shared" si="9"/>
-        <v>-57864.715380899404</v>
+        <v>-32173.019044068453</v>
       </c>
       <c r="X7" s="11">
         <f t="shared" si="1"/>
-        <v>8075.2846191005956</v>
+        <v>33766.980955931547</v>
       </c>
       <c r="Y7" s="11">
         <f t="shared" si="10"/>
-        <v>-62004.715380899404</v>
+        <v>-36313.019044068453</v>
       </c>
       <c r="Z7" s="11">
         <f t="shared" si="11"/>
-        <v>-59628.715380899404</v>
+        <v>-33937.019044068453</v>
       </c>
       <c r="AA7" s="11">
         <f t="shared" si="12"/>
-        <v>-264.71538089940441</v>
+        <v>25426.980955931547</v>
       </c>
       <c r="AB7" s="11">
         <f t="shared" si="13"/>
@@ -17604,27 +17591,27 @@
       </c>
       <c r="AC7" s="12">
         <f t="shared" si="14"/>
-        <v>-37576.118981502368</v>
+        <v>-21623.596900403252</v>
       </c>
       <c r="AD7" s="12">
         <f t="shared" si="15"/>
-        <v>-35929.43563274949</v>
+        <v>-19976.91355165037</v>
       </c>
       <c r="AE7" s="12">
         <f t="shared" si="16"/>
-        <v>5014.1164097711853</v>
+        <v>20966.638490870304</v>
       </c>
       <c r="AF7" s="12">
         <f t="shared" si="17"/>
-        <v>-38500.049910214395</v>
+        <v>-22547.527829115272</v>
       </c>
       <c r="AG7" s="12">
         <f t="shared" si="18"/>
-        <v>-37024.740846625842</v>
+        <v>-21072.218765526723</v>
       </c>
       <c r="AH7" s="12">
         <f t="shared" si="19"/>
-        <v>-164.36742454216633</v>
+        <v>15788.154656556952</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -17684,31 +17671,31 @@
       </c>
       <c r="U8" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V8" s="11">
         <f t="shared" si="8"/>
-        <v>-55128.715380899404</v>
+        <v>-29437.019044068453</v>
       </c>
       <c r="W8" s="11">
         <f t="shared" si="9"/>
-        <v>-50676.715380899404</v>
+        <v>-24985.019044068453</v>
       </c>
       <c r="X8" s="11">
         <f t="shared" si="1"/>
-        <v>81683.284619100596</v>
+        <v>107374.98095593155</v>
       </c>
       <c r="Y8" s="11">
         <f t="shared" si="10"/>
-        <v>-57132.715380899404</v>
+        <v>-31441.019044068453</v>
       </c>
       <c r="Z8" s="11">
         <f t="shared" si="11"/>
-        <v>-53136.715380899404</v>
+        <v>-27445.019044068453</v>
       </c>
       <c r="AA8" s="11">
         <f t="shared" si="12"/>
-        <v>65975.284619100596</v>
+        <v>91666.980955931547</v>
       </c>
       <c r="AB8" s="11">
         <f t="shared" si="13"/>
@@ -17716,27 +17703,27 @@
       </c>
       <c r="AC8" s="12">
         <f t="shared" si="14"/>
-        <v>-31118.722629872402</v>
+        <v>-16616.429828873202</v>
       </c>
       <c r="AD8" s="12">
         <f t="shared" si="15"/>
-        <v>-28605.684693272986</v>
+        <v>-14103.391892273787</v>
       </c>
       <c r="AE8" s="12">
         <f t="shared" si="16"/>
-        <v>46108.084688644965</v>
+        <v>60610.377489644168</v>
       </c>
       <c r="AF8" s="12">
         <f t="shared" si="17"/>
-        <v>-32249.928385700172</v>
+        <v>-17747.635584700973</v>
       </c>
       <c r="AG8" s="12">
         <f t="shared" si="18"/>
-        <v>-29994.290561205278</v>
+        <v>-15491.997760206079</v>
       </c>
       <c r="AH8" s="12">
         <f t="shared" si="19"/>
-        <v>37241.328195360235</v>
+        <v>51743.62099635943</v>
       </c>
     </row>
     <row r="9" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -17795,31 +17782,31 @@
       </c>
       <c r="U9" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V9" s="11">
         <f t="shared" si="8"/>
-        <v>-47796.715380899404</v>
+        <v>-22105.019044068453</v>
       </c>
       <c r="W9" s="11">
         <f t="shared" si="9"/>
-        <v>-40584.715380899404</v>
+        <v>-14893.019044068453</v>
       </c>
       <c r="X9" s="11">
         <f t="shared" si="1"/>
-        <v>206627.2846191006</v>
+        <v>232318.98095593153</v>
       </c>
       <c r="Y9" s="11">
         <f t="shared" si="10"/>
-        <v>-50544.715380899404</v>
+        <v>-24853.019044068453</v>
       </c>
       <c r="Z9" s="11">
         <f t="shared" si="11"/>
-        <v>-44064.715380899404</v>
+        <v>-18373.019044068453</v>
       </c>
       <c r="AA9" s="11">
         <f t="shared" si="12"/>
-        <v>178451.2846191006</v>
+        <v>204142.98095593153</v>
       </c>
       <c r="AB9" s="11">
         <f t="shared" si="13"/>
@@ -17827,27 +17814,27 @@
       </c>
       <c r="AC9" s="12">
         <f t="shared" si="14"/>
-        <v>-24527.272522471001</v>
+        <v>-11343.369976108097</v>
       </c>
       <c r="AD9" s="12">
         <f t="shared" si="15"/>
-        <v>-20826.376173791148</v>
+        <v>-7642.4736274282423</v>
       </c>
       <c r="AE9" s="12">
         <f t="shared" si="16"/>
-        <v>106032.46855025826</v>
+        <v>119216.37109662115</v>
       </c>
       <c r="AF9" s="12">
         <f t="shared" si="17"/>
-        <v>-25937.431031368982</v>
+        <v>-12753.528485006078</v>
       </c>
       <c r="AG9" s="12">
         <f t="shared" si="18"/>
-        <v>-22612.166425234005</v>
+        <v>-9428.263878871101</v>
       </c>
       <c r="AH9" s="12">
         <f t="shared" si="19"/>
-        <v>91573.725410989864</v>
+        <v>104757.62795735277</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -17906,31 +17893,31 @@
       </c>
       <c r="U10" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V10" s="11">
         <f t="shared" si="8"/>
-        <v>-37812.715380899404</v>
+        <v>-12121.019044068453</v>
       </c>
       <c r="W10" s="11">
         <f t="shared" si="9"/>
-        <v>-26472.715380899404</v>
+        <v>-781.01904406845279</v>
       </c>
       <c r="X10" s="11">
         <f t="shared" si="1"/>
-        <v>387911.28461910062</v>
+        <v>413602.98095593153</v>
       </c>
       <c r="Y10" s="11">
         <f t="shared" si="10"/>
-        <v>-41580.715380899404</v>
+        <v>-15889.019044068453</v>
       </c>
       <c r="Z10" s="11">
         <f t="shared" si="11"/>
-        <v>-31368.715380899404</v>
+        <v>-5677.0190440684528</v>
       </c>
       <c r="AA10" s="11">
         <f t="shared" si="12"/>
-        <v>341567.28461910062</v>
+        <v>367258.98095593153</v>
       </c>
       <c r="AB10" s="11">
         <f t="shared" si="13"/>
@@ -17938,27 +17925,27 @@
       </c>
       <c r="AC10" s="12">
         <f t="shared" si="14"/>
-        <v>-17639.910790959664</v>
+        <v>-5654.5448397206583</v>
       </c>
       <c r="AD10" s="12">
         <f t="shared" si="15"/>
-        <v>-12349.717099381289</v>
+        <v>-364.35114814228405</v>
       </c>
       <c r="AE10" s="12">
         <f t="shared" si="16"/>
-        <v>180963.47714144879</v>
+        <v>192948.84309268778</v>
       </c>
       <c r="AF10" s="12">
         <f t="shared" si="17"/>
-        <v>-19397.710599589936</v>
+        <v>-7412.3446483509324</v>
       </c>
       <c r="AG10" s="12">
         <f t="shared" si="18"/>
-        <v>-14633.737232888143</v>
+        <v>-2648.3712816491375</v>
       </c>
       <c r="AH10" s="12">
         <f t="shared" si="19"/>
-        <v>159343.65911300891</v>
+        <v>171329.02506424789</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18017,31 +18004,31 @@
       </c>
       <c r="U11" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V11" s="11">
         <f t="shared" si="8"/>
-        <v>-24348.715380899404</v>
+        <v>1342.9809559315472</v>
       </c>
       <c r="W11" s="11">
         <f t="shared" si="9"/>
-        <v>-6924.7153808994044</v>
+        <v>18766.980955931547</v>
       </c>
       <c r="X11" s="11">
         <f t="shared" si="1"/>
-        <v>581603.28461910062</v>
+        <v>607294.98095593159</v>
       </c>
       <c r="Y11" s="11">
         <f t="shared" si="10"/>
-        <v>-29436.715380899404</v>
+        <v>-3745.0190440684528</v>
       </c>
       <c r="Z11" s="11">
         <f t="shared" si="11"/>
-        <v>-13752.715380899404</v>
+        <v>11938.980955931547</v>
       </c>
       <c r="AA11" s="11">
         <f t="shared" si="12"/>
-        <v>515891.28461910062</v>
+        <v>541582.98095593159</v>
       </c>
       <c r="AB11" s="11">
         <f t="shared" si="13"/>
@@ -18049,27 +18036,27 @@
       </c>
       <c r="AC11" s="12">
         <f t="shared" si="14"/>
-        <v>-10326.232203468922</v>
+        <v>569.55502493017195</v>
       </c>
       <c r="AD11" s="12">
         <f t="shared" si="15"/>
-        <v>-2936.7553009467506</v>
+        <v>7959.0319274523445</v>
       </c>
       <c r="AE11" s="12">
         <f t="shared" si="16"/>
-        <v>246656.56784457492</v>
+        <v>257552.35507297402</v>
       </c>
       <c r="AF11" s="12">
         <f t="shared" si="17"/>
-        <v>-12484.040885748125</v>
+        <v>-1588.2536573490299</v>
       </c>
       <c r="AG11" s="12">
         <f t="shared" si="18"/>
-        <v>-5832.4938391940759</v>
+        <v>5063.2933892050196</v>
       </c>
       <c r="AH11" s="12">
         <f t="shared" si="19"/>
-        <v>218788.26514608221</v>
+        <v>229684.05237448131</v>
       </c>
     </row>
     <row r="12" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18129,31 +18116,31 @@
       </c>
       <c r="U12" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V12" s="11">
         <f t="shared" si="8"/>
-        <v>-6360.7153808994044</v>
+        <v>19330.980955931547</v>
       </c>
       <c r="W12" s="11">
         <f t="shared" si="9"/>
-        <v>19811.284619100596</v>
+        <v>45502.980955931547</v>
       </c>
       <c r="X12" s="11">
         <f t="shared" si="1"/>
-        <v>697895.28461910062</v>
+        <v>723586.98095593159</v>
       </c>
       <c r="Y12" s="11">
         <f t="shared" si="10"/>
-        <v>-13260.715380899404</v>
+        <v>12430.980955931547</v>
       </c>
       <c r="Z12" s="11">
         <f t="shared" si="11"/>
-        <v>10283.284619100596</v>
+        <v>35974.980955931547</v>
       </c>
       <c r="AA12" s="11">
         <f t="shared" si="12"/>
-        <v>620567.28461910062</v>
+        <v>646258.98095593159</v>
       </c>
       <c r="AB12" s="11">
         <f t="shared" si="13"/>
@@ -18161,27 +18148,27 @@
       </c>
       <c r="AC12" s="12">
         <f t="shared" si="14"/>
-        <v>-2452.3311310769718</v>
+        <v>7452.9299856494772</v>
       </c>
       <c r="AD12" s="12">
         <f t="shared" si="15"/>
-        <v>7638.1078398727259</v>
+        <v>17543.368956599177</v>
       </c>
       <c r="AE12" s="12">
         <f t="shared" si="16"/>
-        <v>269068.84370940714</v>
+        <v>278974.10482613364</v>
       </c>
       <c r="AF12" s="12">
         <f t="shared" si="17"/>
-        <v>-5112.5798281407388</v>
+        <v>4792.6812885857107</v>
       </c>
       <c r="AG12" s="12">
         <f t="shared" si="18"/>
-        <v>3964.6513781881504</v>
+        <v>13869.912494914599</v>
       </c>
       <c r="AH12" s="12">
         <f t="shared" si="19"/>
-        <v>239255.55222440034</v>
+        <v>249160.81334112681</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18240,31 +18227,31 @@
       </c>
       <c r="U13" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V13" s="11">
         <f t="shared" si="8"/>
-        <v>17447.284619100596</v>
+        <v>43138.980955931547</v>
       </c>
       <c r="W13" s="11">
         <f t="shared" si="9"/>
-        <v>55679.284619100596</v>
+        <v>81370.980955931547</v>
       </c>
       <c r="X13" s="11">
         <f t="shared" si="1"/>
-        <v>722819.28461910062</v>
+        <v>748510.98095593159</v>
       </c>
       <c r="Y13" s="11">
         <f t="shared" si="10"/>
-        <v>8171.2846191005956</v>
+        <v>33862.980955931547</v>
       </c>
       <c r="Z13" s="11">
         <f t="shared" si="11"/>
-        <v>42575.284619100596</v>
+        <v>68266.980955931547</v>
       </c>
       <c r="AA13" s="11">
         <f t="shared" si="12"/>
-        <v>642995.28461910062</v>
+        <v>668686.98095593159</v>
       </c>
       <c r="AB13" s="11">
         <f t="shared" si="13"/>
@@ -18272,27 +18259,27 @@
       </c>
       <c r="AC13" s="12">
         <f t="shared" si="14"/>
-        <v>6115.1668215102845</v>
+        <v>15119.949654897964</v>
       </c>
       <c r="AD13" s="12">
         <f t="shared" si="15"/>
-        <v>19515.249586482871</v>
+        <v>28520.032419870549</v>
       </c>
       <c r="AE13" s="12">
         <f t="shared" si="16"/>
-        <v>253343.74968649886</v>
+        <v>262348.53251988656</v>
       </c>
       <c r="AF13" s="12">
         <f t="shared" si="17"/>
-        <v>2863.9854099208901</v>
+        <v>11868.76824330857</v>
       </c>
       <c r="AG13" s="12">
         <f t="shared" si="18"/>
-        <v>14922.377527678707</v>
+        <v>23927.160361066388</v>
       </c>
       <c r="AH13" s="12">
         <f t="shared" si="19"/>
-        <v>225365.92465429622</v>
+        <v>234370.70748768392</v>
       </c>
     </row>
     <row r="14" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18351,31 +18338,31 @@
       </c>
       <c r="U14" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V14" s="11">
         <f t="shared" si="8"/>
-        <v>48443.284619100596</v>
+        <v>74134.980955931547</v>
       </c>
       <c r="W14" s="11">
         <f t="shared" si="9"/>
-        <v>102587.2846191006</v>
+        <v>128278.98095593155</v>
       </c>
       <c r="X14" s="11">
         <f t="shared" si="1"/>
-        <v>723983.28461910062</v>
+        <v>749674.98095593159</v>
       </c>
       <c r="Y14" s="11">
         <f t="shared" si="10"/>
-        <v>36071.284619100596</v>
+        <v>61762.980955931547</v>
       </c>
       <c r="Z14" s="11">
         <f t="shared" si="11"/>
-        <v>84803.284619100596</v>
+        <v>110494.98095593155</v>
       </c>
       <c r="AA14" s="11">
         <f t="shared" si="12"/>
-        <v>644039.28461910062</v>
+        <v>669730.98095593159</v>
       </c>
       <c r="AB14" s="11">
         <f t="shared" si="13"/>
@@ -18383,27 +18370,27 @@
       </c>
       <c r="AC14" s="12">
         <f t="shared" si="14"/>
-        <v>15435.523390759561</v>
+        <v>23621.689602930179</v>
       </c>
       <c r="AD14" s="12">
         <f t="shared" si="15"/>
-        <v>32687.470384869106</v>
+        <v>40873.636597039724</v>
       </c>
       <c r="AE14" s="12">
         <f t="shared" si="16"/>
-        <v>230683.38598681384</v>
+        <v>238869.55219898446</v>
       </c>
       <c r="AF14" s="12">
         <f t="shared" si="17"/>
-        <v>11493.422914047031</v>
+        <v>19679.589126217648</v>
       </c>
       <c r="AG14" s="12">
         <f t="shared" si="18"/>
-        <v>27020.939922708127</v>
+        <v>35207.106134878748</v>
       </c>
       <c r="AH14" s="12">
         <f t="shared" si="19"/>
-        <v>205210.76389577711</v>
+        <v>213396.93010794773</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18462,31 +18449,31 @@
       </c>
       <c r="U15" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V15" s="11">
         <f t="shared" si="8"/>
-        <v>88043.284619100596</v>
+        <v>113734.98095593155</v>
       </c>
       <c r="W15" s="11">
         <f t="shared" si="9"/>
-        <v>161807.2846191006</v>
+        <v>187498.98095593153</v>
       </c>
       <c r="X15" s="11">
         <f t="shared" si="1"/>
-        <v>724151.28461910062</v>
+        <v>749842.98095593159</v>
       </c>
       <c r="Y15" s="11">
         <f t="shared" si="10"/>
-        <v>71699.284619100596</v>
+        <v>97390.980955931547</v>
       </c>
       <c r="Z15" s="11">
         <f t="shared" si="11"/>
-        <v>138107.2846191006</v>
+        <v>163798.98095593153</v>
       </c>
       <c r="AA15" s="11">
         <f t="shared" si="12"/>
-        <v>644195.28461910062</v>
+        <v>669886.98095593159</v>
       </c>
       <c r="AB15" s="11">
         <f t="shared" si="13"/>
@@ -18494,27 +18481,27 @@
       </c>
       <c r="AC15" s="12">
         <f t="shared" si="14"/>
-        <v>25503.003429172437</v>
+        <v>32944.972712963907</v>
       </c>
       <c r="AD15" s="12">
         <f t="shared" si="15"/>
-        <v>46869.806736069477</v>
+        <v>54311.776019860947</v>
       </c>
       <c r="AE15" s="12">
         <f t="shared" si="16"/>
-        <v>209760.83269471745</v>
+        <v>217202.80197850891</v>
       </c>
       <c r="AF15" s="12">
         <f t="shared" si="17"/>
-        <v>20768.728806756015</v>
+        <v>28210.698090547485</v>
       </c>
       <c r="AG15" s="12">
         <f t="shared" si="18"/>
-        <v>40004.760936309976</v>
+        <v>47446.730220101446</v>
       </c>
       <c r="AH15" s="12">
         <f t="shared" si="19"/>
-        <v>186600.42754849084</v>
+        <v>194042.39683228231</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18573,31 +18560,31 @@
       </c>
       <c r="U16" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V16" s="11">
         <f t="shared" si="8"/>
-        <v>137255.2846191006</v>
+        <v>162946.98095593153</v>
       </c>
       <c r="W16" s="11">
         <f t="shared" si="9"/>
-        <v>233303.2846191006</v>
+        <v>258994.98095593153</v>
       </c>
       <c r="X16" s="11">
         <f t="shared" si="1"/>
-        <v>724271.28461910062</v>
+        <v>749962.98095593159</v>
       </c>
       <c r="Y16" s="11">
         <f t="shared" si="10"/>
-        <v>115979.2846191006</v>
+        <v>141670.98095593153</v>
       </c>
       <c r="Z16" s="11">
         <f t="shared" si="11"/>
-        <v>202427.2846191006</v>
+        <v>228118.98095593153</v>
       </c>
       <c r="AA16" s="11">
         <f t="shared" si="12"/>
-        <v>644303.28461910062</v>
+        <v>669994.98095593159</v>
       </c>
       <c r="AB16" s="11">
         <f t="shared" si="13"/>
@@ -18605,27 +18592,27 @@
       </c>
       <c r="AC16" s="12">
         <f t="shared" si="14"/>
-        <v>36143.606258885731</v>
+        <v>42909.032880514336</v>
       </c>
       <c r="AD16" s="12">
         <f t="shared" si="15"/>
-        <v>61436.04657247608</v>
+        <v>68201.473194104678</v>
       </c>
       <c r="AE16" s="12">
         <f t="shared" si="16"/>
-        <v>190723.26583662344</v>
+        <v>197488.69245825204</v>
       </c>
       <c r="AF16" s="12">
         <f t="shared" si="17"/>
-        <v>30540.970492269582</v>
+        <v>37306.397113898187</v>
       </c>
       <c r="AG16" s="12">
         <f t="shared" si="18"/>
-        <v>53305.430764521559</v>
+        <v>60070.857386150165</v>
       </c>
       <c r="AH16" s="12">
         <f t="shared" si="19"/>
-        <v>169665.19209227487</v>
+        <v>176430.61871390347</v>
       </c>
     </row>
     <row r="17" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18684,31 +18671,31 @@
       </c>
       <c r="U17" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V17" s="11">
         <f t="shared" si="8"/>
-        <v>196331.2846191006</v>
+        <v>222022.98095593153</v>
       </c>
       <c r="W17" s="11">
         <f t="shared" si="9"/>
-        <v>314543.28461910062</v>
+        <v>340234.98095593153</v>
       </c>
       <c r="X17" s="11">
         <f t="shared" si="1"/>
-        <v>724319.28461910062</v>
+        <v>750010.98095593159</v>
       </c>
       <c r="Y17" s="11">
         <f t="shared" si="10"/>
-        <v>169151.2846191006</v>
+        <v>194842.98095593153</v>
       </c>
       <c r="Z17" s="11">
         <f t="shared" si="11"/>
-        <v>275555.28461910062</v>
+        <v>301246.98095593153</v>
       </c>
       <c r="AA17" s="11">
         <f t="shared" si="12"/>
-        <v>644351.28461910062</v>
+        <v>670042.98095593159</v>
       </c>
       <c r="AB17" s="11">
         <f t="shared" si="13"/>
@@ -18716,27 +18703,27 @@
       </c>
       <c r="AC17" s="12">
         <f t="shared" si="14"/>
-        <v>47000.148580246998</v>
+        <v>53150.536418091186</v>
       </c>
       <c r="AD17" s="12">
         <f t="shared" si="15"/>
-        <v>75299.161520274545</v>
+        <v>81449.549358118733</v>
       </c>
       <c r="AE17" s="12">
         <f t="shared" si="16"/>
-        <v>173396.27794257284</v>
+        <v>179546.66578041704</v>
       </c>
       <c r="AF17" s="12">
         <f t="shared" si="17"/>
-        <v>40493.47267839314</v>
+        <v>46643.860516237321</v>
       </c>
       <c r="AG17" s="12">
         <f t="shared" si="18"/>
-        <v>65965.744299469603</v>
+        <v>72116.132137313791</v>
       </c>
       <c r="AH17" s="12">
         <f t="shared" si="19"/>
-        <v>154252.57453861958</v>
+        <v>160402.96237646378</v>
       </c>
     </row>
     <row r="18" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18795,31 +18782,31 @@
       </c>
       <c r="U18" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V18" s="11">
         <f t="shared" si="8"/>
-        <v>264287.28461910062</v>
+        <v>289978.98095593153</v>
       </c>
       <c r="W18" s="11">
         <f t="shared" si="9"/>
-        <v>400199.28461910062</v>
+        <v>425890.98095593153</v>
       </c>
       <c r="X18" s="11">
         <f t="shared" si="1"/>
-        <v>724343.28461910062</v>
+        <v>750034.98095593159</v>
       </c>
       <c r="Y18" s="11">
         <f t="shared" si="10"/>
-        <v>230315.2846191006</v>
+        <v>256006.98095593153</v>
       </c>
       <c r="Z18" s="11">
         <f t="shared" si="11"/>
-        <v>352655.28461910062</v>
+        <v>378346.98095593153</v>
       </c>
       <c r="AA18" s="11">
         <f t="shared" si="12"/>
-        <v>644363.28461910062</v>
+        <v>670054.98095593159</v>
       </c>
       <c r="AB18" s="11">
         <f t="shared" si="13"/>
@@ -18827,27 +18814,27 @@
       </c>
       <c r="AC18" s="12">
         <f t="shared" si="14"/>
-        <v>57516.613351979882</v>
+        <v>63107.875022747321</v>
       </c>
       <c r="AD18" s="12">
         <f t="shared" si="15"/>
-        <v>87095.024455490551</v>
+        <v>92686.286126257983</v>
       </c>
       <c r="AE18" s="12">
         <f t="shared" si="16"/>
-        <v>157638.20304705246</v>
+        <v>163229.46471781991</v>
       </c>
       <c r="AF18" s="12">
         <f t="shared" si="17"/>
-        <v>50123.316350916954</v>
+        <v>55714.578021684392</v>
       </c>
       <c r="AG18" s="12">
         <f t="shared" si="18"/>
-        <v>76748.064823483728</v>
+        <v>82339.32649425116</v>
       </c>
       <c r="AH18" s="12">
         <f t="shared" si="19"/>
-        <v>140232.22476655638</v>
+        <v>145823.48643732382</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18897,31 +18884,31 @@
       </c>
       <c r="U19" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V19" s="11">
         <f t="shared" si="8"/>
-        <v>338339.28461910062</v>
+        <v>364030.98095593153</v>
       </c>
       <c r="W19" s="11">
         <f t="shared" si="9"/>
-        <v>482855.28461910062</v>
+        <v>508546.98095593153</v>
       </c>
       <c r="X19" s="11">
         <f t="shared" si="1"/>
-        <v>724355.28461910062</v>
+        <v>750046.98095593159</v>
       </c>
       <c r="Y19" s="11">
         <f t="shared" si="10"/>
-        <v>296951.28461910062</v>
+        <v>322642.98095593153</v>
       </c>
       <c r="Z19" s="11">
         <f t="shared" si="11"/>
-        <v>427031.28461910062</v>
+        <v>452722.98095593153</v>
       </c>
       <c r="AA19" s="11">
         <f t="shared" si="12"/>
-        <v>644375.28461910062</v>
+        <v>670066.98095593159</v>
       </c>
       <c r="AB19" s="11">
         <f t="shared" si="13"/>
@@ -18929,27 +18916,27 @@
       </c>
       <c r="AC19" s="12">
         <f t="shared" si="14"/>
-        <v>66938.623741374511</v>
+        <v>72021.588896617628</v>
       </c>
       <c r="AD19" s="12">
         <f t="shared" si="15"/>
-        <v>95530.343912146418</v>
+        <v>100613.30906738955</v>
       </c>
       <c r="AE19" s="12">
         <f t="shared" si="16"/>
-        <v>143309.83145152903</v>
+        <v>148392.79660677217</v>
       </c>
       <c r="AF19" s="12">
         <f t="shared" si="17"/>
-        <v>58750.228584935721</v>
+        <v>63833.193740178845</v>
       </c>
       <c r="AG19" s="12">
         <f t="shared" si="18"/>
-        <v>84485.863115465283</v>
+        <v>89568.828270708414</v>
       </c>
       <c r="AH19" s="12">
         <f t="shared" si="19"/>
-        <v>127486.21483289624</v>
+        <v>132569.17998813937</v>
       </c>
     </row>
     <row r="20" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18999,31 +18986,31 @@
       </c>
       <c r="U20" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V20" s="11">
         <f t="shared" si="8"/>
-        <v>413975.28461910062</v>
+        <v>439666.98095593153</v>
       </c>
       <c r="W20" s="11">
         <f t="shared" si="9"/>
-        <v>555143.28461910062</v>
+        <v>580834.98095593159</v>
       </c>
       <c r="X20" s="11">
         <f t="shared" si="1"/>
-        <v>724403.28461910062</v>
+        <v>750094.98095593159</v>
       </c>
       <c r="Y20" s="11">
         <f t="shared" si="10"/>
-        <v>365051.28461910062</v>
+        <v>390742.98095593153</v>
       </c>
       <c r="Z20" s="11">
         <f t="shared" si="11"/>
-        <v>492083.28461910062</v>
+        <v>517774.98095593153</v>
       </c>
       <c r="AA20" s="11">
         <f t="shared" si="12"/>
-        <v>644423.28461910062</v>
+        <v>670114.98095593159</v>
       </c>
       <c r="AB20" s="11">
         <f t="shared" si="13"/>
@@ -19031,27 +19018,27 @@
       </c>
       <c r="AC20" s="12">
         <f t="shared" si="14"/>
-        <v>74457.093743913734</v>
+        <v>79077.971157771128</v>
       </c>
       <c r="AD20" s="12">
         <f t="shared" si="15"/>
-        <v>99847.399397817615</v>
+        <v>104468.27681167501</v>
       </c>
       <c r="AE20" s="12">
         <f t="shared" si="16"/>
-        <v>130290.29817785112</v>
+        <v>134911.17559170851</v>
       </c>
       <c r="AF20" s="12">
         <f t="shared" si="17"/>
-        <v>65657.682306395378</v>
+        <v>70278.559720252757</v>
       </c>
       <c r="AG20" s="12">
         <f t="shared" si="18"/>
-        <v>88505.504106142602</v>
+        <v>93126.381519999981</v>
       </c>
       <c r="AH20" s="12">
         <f t="shared" si="19"/>
-        <v>115905.19216091221</v>
+        <v>120526.0695747696</v>
       </c>
     </row>
     <row r="21" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19101,31 +19088,31 @@
       </c>
       <c r="U21" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V21" s="11">
         <f t="shared" si="8"/>
-        <v>485939.28461910062</v>
+        <v>511630.98095593153</v>
       </c>
       <c r="W21" s="11">
         <f t="shared" si="9"/>
-        <v>612371.28461910062</v>
+        <v>638062.98095593159</v>
       </c>
       <c r="X21" s="11">
         <f t="shared" si="1"/>
-        <v>724415.28461910062</v>
+        <v>750106.98095593159</v>
       </c>
       <c r="Y21" s="11">
         <f t="shared" si="10"/>
-        <v>429803.28461910062</v>
+        <v>455494.98095593153</v>
       </c>
       <c r="Z21" s="11">
         <f t="shared" si="11"/>
-        <v>543587.28461910062</v>
+        <v>569278.98095593159</v>
       </c>
       <c r="AA21" s="11">
         <f t="shared" si="12"/>
-        <v>644435.28461910062</v>
+        <v>670126.98095593159</v>
       </c>
       <c r="AB21" s="11">
         <f t="shared" si="13"/>
@@ -19133,27 +19120,27 @@
       </c>
       <c r="AC21" s="12">
         <f t="shared" si="14"/>
-        <v>79454.956091763976</v>
+        <v>83655.753740725224</v>
       </c>
       <c r="AD21" s="12">
         <f t="shared" si="15"/>
-        <v>100127.59838794734</v>
+        <v>104328.3960369086</v>
       </c>
       <c r="AE21" s="12">
         <f t="shared" si="16"/>
-        <v>118447.68771211818</v>
+        <v>122648.48536107944</v>
       </c>
       <c r="AF21" s="12">
         <f t="shared" si="17"/>
-        <v>70276.271518724316</v>
+        <v>74477.069167685579</v>
       </c>
       <c r="AG21" s="12">
         <f t="shared" si="18"/>
-        <v>88880.864746933381</v>
+        <v>93081.662395894644</v>
       </c>
       <c r="AH21" s="12">
         <f t="shared" si="19"/>
-        <v>105370.31860581008</v>
+        <v>109571.11625477135</v>
       </c>
     </row>
     <row r="22" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19203,31 +19190,31 @@
       </c>
       <c r="U22" s="7">
         <f>OPEX!$B$15</f>
-        <v>75132.715380899404</v>
+        <v>49441.019044068453</v>
       </c>
       <c r="V22" s="11">
         <f t="shared" si="8"/>
-        <v>549371.28461910062</v>
+        <v>575062.98095593159</v>
       </c>
       <c r="W22" s="11">
         <f t="shared" si="9"/>
-        <v>653687.28461910062</v>
+        <v>679378.98095593159</v>
       </c>
       <c r="X22" s="11">
         <f t="shared" si="1"/>
-        <v>724415.28461910062</v>
+        <v>750106.98095593159</v>
       </c>
       <c r="Y22" s="11">
         <f t="shared" si="10"/>
-        <v>486899.28461910062</v>
+        <v>512590.98095593153</v>
       </c>
       <c r="Z22" s="11">
         <f t="shared" si="11"/>
-        <v>580787.28461910062</v>
+        <v>606478.98095593159</v>
       </c>
       <c r="AA22" s="11">
         <f t="shared" si="12"/>
-        <v>644435.28461910062</v>
+        <v>670126.98095593159</v>
       </c>
       <c r="AB22" s="11">
         <f t="shared" si="13"/>
@@ -19235,27 +19222,27 @@
       </c>
       <c r="AC22" s="12">
         <f t="shared" si="14"/>
-        <v>81660.540878067462</v>
+        <v>85479.447831668615</v>
       </c>
       <c r="AD22" s="12">
         <f t="shared" si="15"/>
-        <v>97166.449579034015</v>
+        <v>100985.35653263517</v>
       </c>
       <c r="AE22" s="12">
         <f t="shared" si="16"/>
-        <v>107679.71610192563</v>
+        <v>111498.62305552678</v>
       </c>
       <c r="AF22" s="12">
         <f t="shared" si="17"/>
-        <v>72374.476148143163</v>
+        <v>76193.383101744301</v>
       </c>
       <c r="AG22" s="12">
         <f t="shared" si="18"/>
-        <v>86330.329096073954</v>
+        <v>90149.236049675106</v>
       </c>
       <c r="AH22" s="12">
         <f t="shared" si="19"/>
-        <v>95791.198732554636</v>
+        <v>99610.105686155788</v>
       </c>
     </row>
     <row r="25" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19790,7 +19777,7 @@
         <v>46016</v>
       </c>
     </row>
-    <row r="45" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2034</v>
       </c>
@@ -19819,7 +19806,7 @@
         <v>46017</v>
       </c>
     </row>
-    <row r="46" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2035</v>
       </c>
@@ -19848,7 +19835,7 @@
         <v>46018</v>
       </c>
     </row>
-    <row r="47" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2036</v>
       </c>
@@ -19877,7 +19864,7 @@
         <v>46019</v>
       </c>
     </row>
-    <row r="48" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2037</v>
       </c>
@@ -19906,7 +19893,7 @@
         <v>46020</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2038</v>
       </c>
@@ -19935,12 +19922,12 @@
         <v>46020</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -19963,7 +19950,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>2018</v>
       </c>
@@ -19992,7 +19979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>2019</v>
       </c>

</xml_diff>